<commit_message>
Added some design thoughts into OSEK-Builder.py
</commit_message>
<xml_diff>
--- a/tools/OSEK-Builder.xlsx
+++ b/tools/OSEK-Builder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\osex-os\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BC0C9D-9D10-46C5-864E-A3BAC87102B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4462CE8A-132D-4D02-BBBA-3E8E195BDE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t>S.No</t>
   </si>
@@ -197,6 +197,15 @@
   </si>
   <si>
     <t>inter_task_message</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>Provide a meaningful name for the CPU that you are going to use.</t>
+  </si>
+  <si>
+    <t>Intel_x86_64</t>
   </si>
 </sst>
 </file>
@@ -549,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -583,13 +592,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -597,13 +606,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -611,10 +620,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="6" t="b">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>20</v>
@@ -625,7 +634,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="6" t="b">
         <v>0</v>
@@ -639,7 +648,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="6" t="b">
         <v>0</v>
@@ -653,7 +662,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="6" t="b">
         <v>0</v>
@@ -667,7 +676,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="6" t="b">
         <v>0</v>
@@ -681,7 +690,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="6" t="b">
         <v>0</v>
@@ -695,7 +704,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="6" t="b">
         <v>0</v>
@@ -709,12 +718,26 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -727,13 +750,13 @@
           <x14:formula1>
             <xm:f>DataSelections!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C3</xm:sqref>
+          <xm:sqref>C4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D2E54B79-E7B4-4692-A25C-6B1E38D6AF44}">
           <x14:formula1>
             <xm:f>DataSelections!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C4:C11</xm:sqref>
+          <xm:sqref>C5:C12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -808,7 +831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E239873-4C3E-401B-A75E-3BFB38EFA871}">
   <dimension ref="A1:I200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Completed reading OS & CPU OIL inputs
</commit_message>
<xml_diff>
--- a/tools/OSEK-Builder.xlsx
+++ b/tools/OSEK-Builder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\osex-os\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4462CE8A-132D-4D02-BBBA-3E8E195BDE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE36BC3-A89B-4126-83CA-02028927F7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -561,7 +561,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Successfully generated the Oil file from Excel file
</commit_message>
<xml_diff>
--- a/tools/OSEK-Builder.xlsx
+++ b/tools/OSEK-Builder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\osex-os\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE36BC3-A89B-4126-83CA-02028927F7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E10677B-A0E6-454C-80DD-57D078DC11DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>S.No</t>
   </si>
@@ -106,9 +106,6 @@
     <t>USERESSCHEDULER</t>
   </si>
   <si>
-    <t>osek-os</t>
-  </si>
-  <si>
     <t>Give any name for the OS. The executable binary will be generated in this name.</t>
   </si>
   <si>
@@ -190,9 +187,6 @@
     <t>event1</t>
   </si>
   <si>
-    <t>event2</t>
-  </si>
-  <si>
     <t>event1, event2</t>
   </si>
   <si>
@@ -205,7 +199,13 @@
     <t>Provide a meaningful name for the CPU that you are going to use.</t>
   </si>
   <si>
-    <t>Intel_x86_64</t>
+    <t>mutex1</t>
+  </si>
+  <si>
+    <t>osek_os</t>
+  </si>
+  <si>
+    <t>ARM64</t>
   </si>
 </sst>
 </file>
@@ -560,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -592,13 +592,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -609,10 +609,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -623,10 +623,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -640,7 +640,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -654,7 +654,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -668,7 +668,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -682,7 +682,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -696,7 +696,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -710,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -724,7 +724,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -738,7 +738,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -769,7 +769,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -781,10 +781,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -792,7 +792,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -800,7 +800,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -808,7 +808,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25"/>
@@ -831,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E239873-4C3E-401B-A75E-3BFB38EFA871}">
   <dimension ref="A1:I200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -854,28 +854,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="E1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -883,28 +883,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="6">
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="6">
         <v>1</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="I2" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -912,28 +912,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="6">
         <v>1</v>
       </c>
-      <c r="F3" s="6">
-        <v>1</v>
-      </c>
       <c r="G3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -941,13 +935,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="6">
         <v>1</v>
@@ -956,13 +950,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25"/>
@@ -1196,35 +1187,35 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added support for Counter in oil file output
</commit_message>
<xml_diff>
--- a/tools/OSEK-Builder.xlsx
+++ b/tools/OSEK-Builder.xlsx
@@ -8,20 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\osex-os\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E10677B-A0E6-454C-80DD-57D078DC11DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B7A70E-FAC1-42CA-845D-FC562894708D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS" sheetId="1" r:id="rId1"/>
     <sheet name="APPMODE" sheetId="4" r:id="rId2"/>
     <sheet name="TASK" sheetId="3" r:id="rId3"/>
-    <sheet name="DataSelections" sheetId="2" state="hidden" r:id="rId4"/>
+    <sheet name="COUNTER" sheetId="5" r:id="rId4"/>
+    <sheet name="ALARM" sheetId="6" r:id="rId5"/>
+    <sheet name="DataSelections" sheetId="2" state="hidden" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -62,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="78">
   <si>
     <t>S.No</t>
   </si>
@@ -145,15 +156,6 @@
     <t>AUTOSTART</t>
   </si>
   <si>
-    <t>RESOURCE</t>
-  </si>
-  <si>
-    <t>EVENT</t>
-  </si>
-  <si>
-    <t>MESSAGE</t>
-  </si>
-  <si>
     <t>Task_A</t>
   </si>
   <si>
@@ -206,6 +208,105 @@
   </si>
   <si>
     <t>ARM64</t>
+  </si>
+  <si>
+    <t>Counter Name</t>
+  </si>
+  <si>
+    <t>MINCYCLE</t>
+  </si>
+  <si>
+    <t>MAXALLOWEDVALUE</t>
+  </si>
+  <si>
+    <t>TICKSPERBASE</t>
+  </si>
+  <si>
+    <t>SystemTick</t>
+  </si>
+  <si>
+    <t>RTC_Tick</t>
+  </si>
+  <si>
+    <t>This will be used for real time clock.</t>
+  </si>
+  <si>
+    <t>0xFFFFFFFF</t>
+  </si>
+  <si>
+    <t>Assuming 24 MHz clock, we need 1µs per tick. This will be mostly used for scheduling and alarms</t>
+  </si>
+  <si>
+    <t>Alarm Name</t>
+  </si>
+  <si>
+    <t>COUNTER</t>
+  </si>
+  <si>
+    <t>ACTION</t>
+  </si>
+  <si>
+    <t>arg1</t>
+  </si>
+  <si>
+    <t>arg2</t>
+  </si>
+  <si>
+    <t>WakeTaskA</t>
+  </si>
+  <si>
+    <t>WakeTaskB</t>
+  </si>
+  <si>
+    <t>RunCallbackC</t>
+  </si>
+  <si>
+    <t>ACTIVATETASK</t>
+  </si>
+  <si>
+    <t>SETEVENT</t>
+  </si>
+  <si>
+    <t>ALARMCALLBACK</t>
+  </si>
+  <si>
+    <t>ALARM-ACTION</t>
+  </si>
+  <si>
+    <t>Action-Type</t>
+  </si>
+  <si>
+    <t>event2</t>
+  </si>
+  <si>
+    <t>clock_minute_callback</t>
+  </si>
+  <si>
+    <t>ALARMTIME</t>
+  </si>
+  <si>
+    <t>CYCLETIME</t>
+  </si>
+  <si>
+    <t>APPMODE[]</t>
+  </si>
+  <si>
+    <t>AUTOSTART[]</t>
+  </si>
+  <si>
+    <t>EVENT[]</t>
+  </si>
+  <si>
+    <t>RESOURCE[]</t>
+  </si>
+  <si>
+    <t>MESSAGE[]</t>
+  </si>
+  <si>
+    <t>1, 2</t>
+  </si>
+  <si>
+    <t>Autostart?</t>
   </si>
 </sst>
 </file>
@@ -248,7 +349,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -256,11 +357,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -277,6 +430,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -592,13 +761,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -609,7 +778,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>14</v>
@@ -781,10 +950,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -792,7 +961,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -800,7 +969,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -808,7 +977,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25"/>
@@ -831,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E239873-4C3E-401B-A75E-3BFB38EFA871}">
   <dimension ref="A1:I200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -843,7 +1012,7 @@
     <col min="4" max="4" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.85546875" style="6" customWidth="1"/>
     <col min="9" max="9" width="27.140625" style="6" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" hidden="1"/>
@@ -866,16 +1035,16 @@
         <v>25</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -883,7 +1052,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" s="6">
         <v>1</v>
@@ -895,16 +1064,16 @@
         <v>1</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -912,7 +1081,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C3" s="6">
         <v>2</v>
@@ -924,10 +1093,13 @@
         <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -935,7 +1107,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -950,10 +1122,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25"/>
@@ -1171,11 +1343,288 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A103A8C4-37CC-4979-8443-ED4B477D0218}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE71126-5246-438C-B5C1-BCB8FD89B9BC}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="88.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>3600</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5079921A-7EDA-4A3F-B050-2BF08026BFFC}">
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.140625" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>50</v>
+      </c>
+      <c r="I4">
+        <v>100</v>
+      </c>
+      <c r="J4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="17" x14ac:dyDescent="0.25"/>
+    <row r="18" x14ac:dyDescent="0.25"/>
+    <row r="19" x14ac:dyDescent="0.25"/>
+    <row r="20" x14ac:dyDescent="0.25"/>
+    <row r="21" x14ac:dyDescent="0.25"/>
+    <row r="22" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="G1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CA721EC2-C77F-4FAA-90D4-A308BF8A7B51}">
+          <x14:formula1>
+            <xm:f>DataSelections!$G$2:$G$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3:D22</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A103A8C4-37CC-4979-8443-ED4B477D0218}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,9 +1632,10 @@
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.140625" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1195,8 +1645,11 @@
       <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -1206,8 +1659,11 @@
       <c r="E2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -1216,6 +1672,14 @@
       </c>
       <c r="E3" t="s">
         <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added support for Alarms in OIL output file
This version supports parsing ALARM data from OSEK-Builder excel
document and generate oil file with alarm as per the format specified in
OSEK bOIL verson 2.5.
</commit_message>
<xml_diff>
--- a/tools/OSEK-Builder.xlsx
+++ b/tools/OSEK-Builder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\osex-os\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B7A70E-FAC1-42CA-845D-FC562894708D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4C214B-4C1D-4D0A-80CB-CE30B839E3C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS" sheetId="1" r:id="rId1"/>
@@ -306,7 +306,7 @@
     <t>1, 2</t>
   </si>
   <si>
-    <t>Autostart?</t>
+    <t>IsAutostart</t>
   </si>
 </sst>
 </file>
@@ -349,7 +349,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -409,11 +409,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -447,6 +473,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1346,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE71126-5246-438C-B5C1-BCB8FD89B9BC}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1433,8 +1461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5079921A-7EDA-4A3F-B050-2BF08026BFFC}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1454,15 +1482,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>55</v>
-      </c>
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
       <c r="D1" s="9" t="s">
         <v>56</v>
       </c>
@@ -1479,9 +1501,15 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
+      <c r="A2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>55</v>
+      </c>
       <c r="D2" s="7" t="s">
         <v>66</v>
       </c>
@@ -1595,11 +1623,8 @@
     <row r="21" x14ac:dyDescent="0.25"/>
     <row r="22" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="3">
     <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="G1:J1"/>
   </mergeCells>

</xml_diff>

<commit_message>
OSEK-builder will use counter names from COUNTER
This version of OSEK-builder will support referencing counters in Alarm
sheet by number. And the OIL file generation will map the number to the
Counter text. Else any change in name needs changes in many sheets of
excel.
</commit_message>
<xml_diff>
--- a/tools/OSEK-Builder.xlsx
+++ b/tools/OSEK-Builder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\osex-os\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4C214B-4C1D-4D0A-80CB-CE30B839E3C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8345C7-590B-4064-B71B-698CE05A4930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="TASK" sheetId="3" r:id="rId3"/>
     <sheet name="COUNTER" sheetId="5" r:id="rId4"/>
     <sheet name="ALARM" sheetId="6" r:id="rId5"/>
-    <sheet name="DataSelections" sheetId="2" state="hidden" r:id="rId6"/>
+    <sheet name="ISR" sheetId="7" r:id="rId6"/>
+    <sheet name="DataSelections" sheetId="2" state="hidden" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -73,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="86">
   <si>
     <t>S.No</t>
   </si>
@@ -225,18 +226,12 @@
     <t>SystemTick</t>
   </si>
   <si>
-    <t>RTC_Tick</t>
-  </si>
-  <si>
     <t>This will be used for real time clock.</t>
   </si>
   <si>
     <t>0xFFFFFFFF</t>
   </si>
   <si>
-    <t>Assuming 24 MHz clock, we need 1µs per tick. This will be mostly used for scheduling and alarms</t>
-  </si>
-  <si>
     <t>Alarm Name</t>
   </si>
   <si>
@@ -258,9 +253,6 @@
     <t>WakeTaskB</t>
   </si>
   <si>
-    <t>RunCallbackC</t>
-  </si>
-  <si>
     <t>ACTIVATETASK</t>
   </si>
   <si>
@@ -276,12 +268,6 @@
     <t>Action-Type</t>
   </si>
   <si>
-    <t>event2</t>
-  </si>
-  <si>
-    <t>clock_minute_callback</t>
-  </si>
-  <si>
     <t>ALARMTIME</t>
   </si>
   <si>
@@ -307,6 +293,45 @@
   </si>
   <si>
     <t>IsAutostart</t>
+  </si>
+  <si>
+    <t>uSecCounter</t>
+  </si>
+  <si>
+    <t>1ms tick, used for scheduling</t>
+  </si>
+  <si>
+    <t>Triggered by SetRelAlarm() or SetAbsAlarm()</t>
+  </si>
+  <si>
+    <t>Cyclic Alarm</t>
+  </si>
+  <si>
+    <t>Cyclic Alarm - start at 20 ms and repeats every 4 ms</t>
+  </si>
+  <si>
+    <t>uSecAlarm</t>
+  </si>
+  <si>
+    <t>Alarm_uSecAlarm_callback</t>
+  </si>
+  <si>
+    <t>ISR Name</t>
+  </si>
+  <si>
+    <t>CATEGORY</t>
+  </si>
+  <si>
+    <t>RESOURCE</t>
+  </si>
+  <si>
+    <t>MESSAGE</t>
+  </si>
+  <si>
+    <t>SystemTickISR</t>
+  </si>
+  <si>
+    <t>Category 1 don't use OS service (except interrupt enable/disable), but 2 can use OS services.</t>
   </si>
 </sst>
 </file>
@@ -439,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -461,6 +486,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -473,8 +500,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1029,7 +1063,7 @@
   <dimension ref="A1:I200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1063,16 +1097,16 @@
         <v>25</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1097,9 +1131,6 @@
       <c r="G2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>37</v>
-      </c>
       <c r="I2" s="6" t="s">
         <v>39</v>
       </c>
@@ -1124,7 +1155,7 @@
         <v>42</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>39</v>
@@ -1375,17 +1406,17 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="88.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="68.42578125" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
@@ -1396,13 +1427,13 @@
       <c r="B1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="17" t="s">
         <v>48</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1416,17 +1447,17 @@
       <c r="B2" t="s">
         <v>49</v>
       </c>
-      <c r="C2">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2">
-        <v>24</v>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1434,19 +1465,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="2">
+        <v>100</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>50</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>3600</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25"/>
@@ -1461,96 +1492,108 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5079921A-7EDA-4A3F-B050-2BF08026BFFC}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="43.140625" customWidth="1"/>
+    <col min="11" max="11" width="46.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="9" t="s">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="G2" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="K2" s="9"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>59</v>
-      </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" t="s">
-        <v>62</v>
       </c>
       <c r="E3" t="s">
         <v>27</v>
       </c>
       <c r="G3" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1558,30 +1601,24 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>60</v>
-      </c>
-      <c r="C4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" t="s">
-        <v>63</v>
       </c>
       <c r="E4" t="s">
         <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="G4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>50</v>
-      </c>
-      <c r="I4">
-        <v>100</v>
-      </c>
-      <c r="J4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1590,19 +1627,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
         <v>61</v>
       </c>
-      <c r="C5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" t="s">
-        <v>64</v>
-      </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25"/>
@@ -1631,12 +1671,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CA721EC2-C77F-4FAA-90D4-A308BF8A7B51}">
           <x14:formula1>
             <xm:f>DataSelections!$G$2:$G$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:D22</xm:sqref>
+          <xm:sqref>D3:D12 D14:D22</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{33E54921-A9E7-4A5A-989C-9ED3A71887B9}">
+          <x14:formula1>
+            <xm:f>DataSelections!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G3:G22 D13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1645,6 +1691,263 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F7B285A-14DA-46B0-A287-0CFC1CA6530A}">
+  <dimension ref="A1:F201"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="84.7109375" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="17" x14ac:dyDescent="0.25"/>
+    <row r="18" x14ac:dyDescent="0.25"/>
+    <row r="19" x14ac:dyDescent="0.25"/>
+    <row r="20" x14ac:dyDescent="0.25"/>
+    <row r="21" x14ac:dyDescent="0.25"/>
+    <row r="22" x14ac:dyDescent="0.25"/>
+    <row r="23" x14ac:dyDescent="0.25"/>
+    <row r="24" x14ac:dyDescent="0.25"/>
+    <row r="25" x14ac:dyDescent="0.25"/>
+    <row r="26" x14ac:dyDescent="0.25"/>
+    <row r="27" x14ac:dyDescent="0.25"/>
+    <row r="28" x14ac:dyDescent="0.25"/>
+    <row r="29" x14ac:dyDescent="0.25"/>
+    <row r="30" x14ac:dyDescent="0.25"/>
+    <row r="31" x14ac:dyDescent="0.25"/>
+    <row r="32" x14ac:dyDescent="0.25"/>
+    <row r="33" x14ac:dyDescent="0.25"/>
+    <row r="34" x14ac:dyDescent="0.25"/>
+    <row r="35" x14ac:dyDescent="0.25"/>
+    <row r="36" x14ac:dyDescent="0.25"/>
+    <row r="37" x14ac:dyDescent="0.25"/>
+    <row r="38" x14ac:dyDescent="0.25"/>
+    <row r="39" x14ac:dyDescent="0.25"/>
+    <row r="40" x14ac:dyDescent="0.25"/>
+    <row r="41" x14ac:dyDescent="0.25"/>
+    <row r="42" x14ac:dyDescent="0.25"/>
+    <row r="43" x14ac:dyDescent="0.25"/>
+    <row r="44" x14ac:dyDescent="0.25"/>
+    <row r="45" x14ac:dyDescent="0.25"/>
+    <row r="46" x14ac:dyDescent="0.25"/>
+    <row r="47" x14ac:dyDescent="0.25"/>
+    <row r="48" x14ac:dyDescent="0.25"/>
+    <row r="49" x14ac:dyDescent="0.25"/>
+    <row r="50" x14ac:dyDescent="0.25"/>
+    <row r="51" x14ac:dyDescent="0.25"/>
+    <row r="52" x14ac:dyDescent="0.25"/>
+    <row r="53" x14ac:dyDescent="0.25"/>
+    <row r="54" x14ac:dyDescent="0.25"/>
+    <row r="55" x14ac:dyDescent="0.25"/>
+    <row r="56" x14ac:dyDescent="0.25"/>
+    <row r="57" x14ac:dyDescent="0.25"/>
+    <row r="58" x14ac:dyDescent="0.25"/>
+    <row r="59" x14ac:dyDescent="0.25"/>
+    <row r="60" x14ac:dyDescent="0.25"/>
+    <row r="61" x14ac:dyDescent="0.25"/>
+    <row r="62" x14ac:dyDescent="0.25"/>
+    <row r="63" x14ac:dyDescent="0.25"/>
+    <row r="64" x14ac:dyDescent="0.25"/>
+    <row r="65" x14ac:dyDescent="0.25"/>
+    <row r="66" x14ac:dyDescent="0.25"/>
+    <row r="67" x14ac:dyDescent="0.25"/>
+    <row r="68" x14ac:dyDescent="0.25"/>
+    <row r="69" x14ac:dyDescent="0.25"/>
+    <row r="70" x14ac:dyDescent="0.25"/>
+    <row r="71" x14ac:dyDescent="0.25"/>
+    <row r="72" x14ac:dyDescent="0.25"/>
+    <row r="73" x14ac:dyDescent="0.25"/>
+    <row r="74" x14ac:dyDescent="0.25"/>
+    <row r="75" x14ac:dyDescent="0.25"/>
+    <row r="76" x14ac:dyDescent="0.25"/>
+    <row r="77" x14ac:dyDescent="0.25"/>
+    <row r="78" x14ac:dyDescent="0.25"/>
+    <row r="79" x14ac:dyDescent="0.25"/>
+    <row r="80" x14ac:dyDescent="0.25"/>
+    <row r="81" x14ac:dyDescent="0.25"/>
+    <row r="82" x14ac:dyDescent="0.25"/>
+    <row r="83" x14ac:dyDescent="0.25"/>
+    <row r="84" x14ac:dyDescent="0.25"/>
+    <row r="85" x14ac:dyDescent="0.25"/>
+    <row r="86" x14ac:dyDescent="0.25"/>
+    <row r="87" x14ac:dyDescent="0.25"/>
+    <row r="88" x14ac:dyDescent="0.25"/>
+    <row r="89" x14ac:dyDescent="0.25"/>
+    <row r="90" x14ac:dyDescent="0.25"/>
+    <row r="91" x14ac:dyDescent="0.25"/>
+    <row r="92" x14ac:dyDescent="0.25"/>
+    <row r="93" x14ac:dyDescent="0.25"/>
+    <row r="94" x14ac:dyDescent="0.25"/>
+    <row r="95" x14ac:dyDescent="0.25"/>
+    <row r="96" x14ac:dyDescent="0.25"/>
+    <row r="97" x14ac:dyDescent="0.25"/>
+    <row r="98" x14ac:dyDescent="0.25"/>
+    <row r="99" x14ac:dyDescent="0.25"/>
+    <row r="100" x14ac:dyDescent="0.25"/>
+    <row r="101" x14ac:dyDescent="0.25"/>
+    <row r="102" x14ac:dyDescent="0.25"/>
+    <row r="103" x14ac:dyDescent="0.25"/>
+    <row r="104" x14ac:dyDescent="0.25"/>
+    <row r="105" x14ac:dyDescent="0.25"/>
+    <row r="106" x14ac:dyDescent="0.25"/>
+    <row r="107" x14ac:dyDescent="0.25"/>
+    <row r="108" x14ac:dyDescent="0.25"/>
+    <row r="109" x14ac:dyDescent="0.25"/>
+    <row r="110" x14ac:dyDescent="0.25"/>
+    <row r="111" x14ac:dyDescent="0.25"/>
+    <row r="112" x14ac:dyDescent="0.25"/>
+    <row r="113" x14ac:dyDescent="0.25"/>
+    <row r="114" x14ac:dyDescent="0.25"/>
+    <row r="115" x14ac:dyDescent="0.25"/>
+    <row r="116" x14ac:dyDescent="0.25"/>
+    <row r="117" x14ac:dyDescent="0.25"/>
+    <row r="118" x14ac:dyDescent="0.25"/>
+    <row r="119" x14ac:dyDescent="0.25"/>
+    <row r="120" x14ac:dyDescent="0.25"/>
+    <row r="121" x14ac:dyDescent="0.25"/>
+    <row r="122" x14ac:dyDescent="0.25"/>
+    <row r="123" x14ac:dyDescent="0.25"/>
+    <row r="124" x14ac:dyDescent="0.25"/>
+    <row r="125" x14ac:dyDescent="0.25"/>
+    <row r="126" x14ac:dyDescent="0.25"/>
+    <row r="127" x14ac:dyDescent="0.25"/>
+    <row r="128" x14ac:dyDescent="0.25"/>
+    <row r="129" x14ac:dyDescent="0.25"/>
+    <row r="130" x14ac:dyDescent="0.25"/>
+    <row r="131" x14ac:dyDescent="0.25"/>
+    <row r="132" x14ac:dyDescent="0.25"/>
+    <row r="133" x14ac:dyDescent="0.25"/>
+    <row r="134" x14ac:dyDescent="0.25"/>
+    <row r="135" x14ac:dyDescent="0.25"/>
+    <row r="136" x14ac:dyDescent="0.25"/>
+    <row r="137" x14ac:dyDescent="0.25"/>
+    <row r="138" x14ac:dyDescent="0.25"/>
+    <row r="139" x14ac:dyDescent="0.25"/>
+    <row r="140" x14ac:dyDescent="0.25"/>
+    <row r="141" x14ac:dyDescent="0.25"/>
+    <row r="142" x14ac:dyDescent="0.25"/>
+    <row r="143" x14ac:dyDescent="0.25"/>
+    <row r="144" x14ac:dyDescent="0.25"/>
+    <row r="145" x14ac:dyDescent="0.25"/>
+    <row r="146" x14ac:dyDescent="0.25"/>
+    <row r="147" x14ac:dyDescent="0.25"/>
+    <row r="148" x14ac:dyDescent="0.25"/>
+    <row r="149" x14ac:dyDescent="0.25"/>
+    <row r="150" x14ac:dyDescent="0.25"/>
+    <row r="151" x14ac:dyDescent="0.25"/>
+    <row r="152" x14ac:dyDescent="0.25"/>
+    <row r="153" x14ac:dyDescent="0.25"/>
+    <row r="154" x14ac:dyDescent="0.25"/>
+    <row r="155" x14ac:dyDescent="0.25"/>
+    <row r="156" x14ac:dyDescent="0.25"/>
+    <row r="157" x14ac:dyDescent="0.25"/>
+    <row r="158" x14ac:dyDescent="0.25"/>
+    <row r="159" x14ac:dyDescent="0.25"/>
+    <row r="160" x14ac:dyDescent="0.25"/>
+    <row r="161" x14ac:dyDescent="0.25"/>
+    <row r="162" x14ac:dyDescent="0.25"/>
+    <row r="163" x14ac:dyDescent="0.25"/>
+    <row r="164" x14ac:dyDescent="0.25"/>
+    <row r="165" x14ac:dyDescent="0.25"/>
+    <row r="166" x14ac:dyDescent="0.25"/>
+    <row r="167" x14ac:dyDescent="0.25"/>
+    <row r="168" x14ac:dyDescent="0.25"/>
+    <row r="169" x14ac:dyDescent="0.25"/>
+    <row r="170" x14ac:dyDescent="0.25"/>
+    <row r="171" x14ac:dyDescent="0.25"/>
+    <row r="172" x14ac:dyDescent="0.25"/>
+    <row r="173" x14ac:dyDescent="0.25"/>
+    <row r="174" x14ac:dyDescent="0.25"/>
+    <row r="175" x14ac:dyDescent="0.25"/>
+    <row r="176" x14ac:dyDescent="0.25"/>
+    <row r="177" x14ac:dyDescent="0.25"/>
+    <row r="178" x14ac:dyDescent="0.25"/>
+    <row r="179" x14ac:dyDescent="0.25"/>
+    <row r="180" x14ac:dyDescent="0.25"/>
+    <row r="181" x14ac:dyDescent="0.25"/>
+    <row r="182" x14ac:dyDescent="0.25"/>
+    <row r="183" x14ac:dyDescent="0.25"/>
+    <row r="184" x14ac:dyDescent="0.25"/>
+    <row r="185" x14ac:dyDescent="0.25"/>
+    <row r="186" x14ac:dyDescent="0.25"/>
+    <row r="187" x14ac:dyDescent="0.25"/>
+    <row r="188" x14ac:dyDescent="0.25"/>
+    <row r="189" x14ac:dyDescent="0.25"/>
+    <row r="190" x14ac:dyDescent="0.25"/>
+    <row r="191" x14ac:dyDescent="0.25"/>
+    <row r="192" x14ac:dyDescent="0.25"/>
+    <row r="193" x14ac:dyDescent="0.25"/>
+    <row r="194" x14ac:dyDescent="0.25"/>
+    <row r="195" x14ac:dyDescent="0.25"/>
+    <row r="196" x14ac:dyDescent="0.25"/>
+    <row r="197" x14ac:dyDescent="0.25"/>
+    <row r="198" x14ac:dyDescent="0.25"/>
+    <row r="199" x14ac:dyDescent="0.25"/>
+    <row r="200" x14ac:dyDescent="0.25"/>
+    <row r="201" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A103A8C4-37CC-4979-8443-ED4B477D0218}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -1671,7 +1974,7 @@
         <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1685,7 +1988,7 @@
         <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1699,12 +2002,12 @@
         <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added support for ISR in OSEK Builder tool
</commit_message>
<xml_diff>
--- a/tools/OSEK-Builder.xlsx
+++ b/tools/OSEK-Builder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\osex-os\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8345C7-590B-4064-B71B-698CE05A4930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595E79A5-D1B4-46FE-867A-B79B6D150AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="85">
   <si>
     <t>S.No</t>
   </si>
@@ -302,9 +302,6 @@
   </si>
   <si>
     <t>Triggered by SetRelAlarm() or SetAbsAlarm()</t>
-  </si>
-  <si>
-    <t>Cyclic Alarm</t>
   </si>
   <si>
     <t>Cyclic Alarm - start at 20 ms and repeats every 4 ms</t>
@@ -1492,8 +1489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5079921A-7EDA-4A3F-B050-2BF08026BFFC}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1593,7 +1590,7 @@
         <v>71</v>
       </c>
       <c r="K3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1619,7 +1616,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1627,7 +1624,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" s="2">
         <v>2</v>
@@ -1636,7 +1633,7 @@
         <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
@@ -1694,8 +1691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F7B285A-14DA-46B0-A287-0CFC1CA6530A}">
   <dimension ref="A1:F201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1714,16 +1711,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -1734,13 +1731,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added support to get 1ms tick for linux_app.
</commit_message>
<xml_diff>
--- a/tools/OSEK-Builder.xlsx
+++ b/tools/OSEK-Builder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\osex-os\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595E79A5-D1B4-46FE-867A-B79B6D150AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC4BAD4-3EC4-4EE2-BF81-B6021F302AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS" sheetId="1" r:id="rId1"/>
@@ -208,9 +208,6 @@
     <t>osek_os</t>
   </si>
   <si>
-    <t>ARM64</t>
-  </si>
-  <si>
     <t>Counter Name</t>
   </si>
   <si>
@@ -329,6 +326,9 @@
   </si>
   <si>
     <t>Category 1 don't use OS service (except interrupt enable/disable), but 2 can use OS services.</t>
+  </si>
+  <si>
+    <t>cortex_m4</t>
   </si>
 </sst>
 </file>
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -823,7 +823,7 @@
         <v>40</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>41</v>
@@ -1094,16 +1094,16 @@
         <v>25</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1422,16 +1422,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="E1" s="17" t="s">
         <v>47</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>48</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -1442,19 +1442,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1462,19 +1462,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" s="2">
         <v>100</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25"/>
@@ -1489,8 +1489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5079921A-7EDA-4A3F-B050-2BF08026BFFC}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1514,7 +1514,7 @@
       <c r="B1" s="9"/>
       <c r="C1" s="15"/>
       <c r="D1" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
@@ -1533,31 +1533,31 @@
         <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>53</v>
-      </c>
       <c r="D2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>65</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>66</v>
       </c>
       <c r="K2" s="11"/>
     </row>
@@ -1566,13 +1566,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
         <v>27</v>
@@ -1587,10 +1587,10 @@
         <v>4</v>
       </c>
       <c r="J3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1598,13 +1598,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
         <v>28</v>
@@ -1616,7 +1616,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1624,22 +1624,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" s="2">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25"/>
@@ -1692,7 +1692,7 @@
   <dimension ref="A1:F201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1711,16 +1711,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -1731,13 +1731,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25"/>
@@ -1971,7 +1971,7 @@
         <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1985,7 +1985,7 @@
         <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1999,12 +1999,12 @@
         <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added TICKDURATION (ns) info in counters
</commit_message>
<xml_diff>
--- a/tools/OSEK-Builder.xlsx
+++ b/tools/OSEK-Builder.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\osex-os\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC4BAD4-3EC4-4EE2-BF81-B6021F302AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05582F39-5F52-470E-8A4E-710FE3A2990F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS" sheetId="1" r:id="rId1"/>
     <sheet name="APPMODE" sheetId="4" r:id="rId2"/>
-    <sheet name="TASK" sheetId="3" r:id="rId3"/>
-    <sheet name="COUNTER" sheetId="5" r:id="rId4"/>
+    <sheet name="COUNTER" sheetId="5" r:id="rId3"/>
+    <sheet name="TASK" sheetId="3" r:id="rId4"/>
     <sheet name="ALARM" sheetId="6" r:id="rId5"/>
     <sheet name="ISR" sheetId="7" r:id="rId6"/>
     <sheet name="DataSelections" sheetId="2" state="hidden" r:id="rId7"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="86">
   <si>
     <t>S.No</t>
   </si>
@@ -220,12 +220,6 @@
     <t>TICKSPERBASE</t>
   </si>
   <si>
-    <t>SystemTick</t>
-  </si>
-  <si>
-    <t>This will be used for real time clock.</t>
-  </si>
-  <si>
     <t>0xFFFFFFFF</t>
   </si>
   <si>
@@ -322,13 +316,22 @@
     <t>MESSAGE</t>
   </si>
   <si>
-    <t>SystemTickISR</t>
-  </si>
-  <si>
     <t>Category 1 don't use OS service (except interrupt enable/disable), but 2 can use OS services.</t>
   </si>
   <si>
     <t>cortex_m4</t>
+  </si>
+  <si>
+    <t>isr_func1</t>
+  </si>
+  <si>
+    <t>This will be used by the users for delays and usec count</t>
+  </si>
+  <si>
+    <t>mSecCounter</t>
+  </si>
+  <si>
+    <t>TICKDURATION (ns)</t>
   </si>
 </sst>
 </file>
@@ -788,7 +791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -823,7 +826,7 @@
         <v>40</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>41</v>
@@ -1056,6 +1059,103 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE71126-5246-438C-B5C1-BCB8FD89B9BC}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="68.42578125" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="2">
+        <v>100</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1000</v>
+      </c>
+      <c r="G3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E239873-4C3E-401B-A75E-3BFB38EFA871}">
   <dimension ref="A1:I200"/>
   <sheetViews>
@@ -1094,16 +1194,16 @@
         <v>25</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="H1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1398,93 +1498,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE71126-5246-438C-B5C1-BCB8FD89B9BC}">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="68.42578125" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="2">
-        <v>100</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5079921A-7EDA-4A3F-B050-2BF08026BFFC}">
   <dimension ref="A1:K22"/>
@@ -1514,7 +1527,7 @@
       <c r="B1" s="9"/>
       <c r="C1" s="15"/>
       <c r="D1" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
@@ -1533,31 +1546,31 @@
         <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="K2" s="11"/>
     </row>
@@ -1566,13 +1579,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
         <v>27</v>
@@ -1587,10 +1600,10 @@
         <v>4</v>
       </c>
       <c r="J3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1598,13 +1611,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
         <v>28</v>
@@ -1616,7 +1629,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1624,22 +1637,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C5" s="2">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25"/>
@@ -1692,7 +1705,7 @@
   <dimension ref="A1:F201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1711,16 +1724,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="E1" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -1737,7 +1750,7 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25"/>
@@ -1971,7 +1984,7 @@
         <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1985,7 +1998,7 @@
         <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1999,12 +2012,12 @@
         <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more constructions (counter, timer, action type args)
</commit_message>
<xml_diff>
--- a/tools/OSEK-Builder.xlsx
+++ b/tools/OSEK-Builder.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\oss\osex-os\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\oss\FreeOSEK\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456D1A1D-822A-4A02-B9E9-9F527D2744C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF5B699-2AF5-49CA-9603-0FB798F7BBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS" sheetId="1" r:id="rId1"/>
@@ -464,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -509,6 +509,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1159,7 +1160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E239873-4C3E-401B-A75E-3BFB38EFA871}">
   <dimension ref="A1:I200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1502,8 +1503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5079921A-7EDA-4A3F-B050-2BF08026BFFC}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1645,7 +1646,7 @@
       <c r="D5" t="s">
         <v>58</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="18" t="s">
         <v>75</v>
       </c>
       <c r="G5" t="b">

</xml_diff>

<commit_message>
Added AppMode code generation for Alarms.
</commit_message>
<xml_diff>
--- a/tools/OSEK-Builder.xlsx
+++ b/tools/OSEK-Builder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\oss\FreeOSEK\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF5B699-2AF5-49CA-9603-0FB798F7BBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0010D7-6E48-47AB-B8EA-320C2CCB4386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -497,6 +497,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -509,7 +510,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1504,7 +1504,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1527,18 +1527,18 @@
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
       <c r="C1" s="11"/>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="15" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="15" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1573,7 +1573,7 @@
       <c r="J2" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="K2" s="14"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -1646,7 +1646,7 @@
       <c r="D5" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="14" t="s">
         <v>75</v>
       </c>
       <c r="G5" t="b">

</xml_diff>

<commit_message>
Tested alarms for OSEK specifications
Configured and reconfigured the OSEK-Builder.xlsx to trigger Task_A for
different timing and found that the scheduling of tasks is happening as
per the design.
</commit_message>
<xml_diff>
--- a/tools/OSEK-Builder.xlsx
+++ b/tools/OSEK-Builder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\oss\FreeOSEK\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0010D7-6E48-47AB-B8EA-320C2CCB4386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E09572C-4F76-4B88-AD93-DA8041A102A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1504,7 +1504,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1598,7 +1598,7 @@
         <v>20</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>500</v>
       </c>
       <c r="J3" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
Redesigned the way the resources are defined.
Earlier the resources were looked from task view point. Now tasks are
viewed from the resources view point. This allows to follow OSEK ceiling
protocol whenever a resources is in use. Else need to loop the task and
find the resource.
</commit_message>
<xml_diff>
--- a/tools/OSEK-Builder.xlsx
+++ b/tools/OSEK-Builder.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aananth/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\oss\FreeOSEK\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05875DA-E4BC-9447-A478-56EC8C84F7C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7872A60-F555-4D3C-BE3D-4DBD0945F3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20740" windowHeight="11320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS" sheetId="1" r:id="rId1"/>
@@ -319,9 +319,6 @@
     <t>Category 1 don't use OS service (except interrupt enable/disable), but 2 can use OS services.</t>
   </si>
   <si>
-    <t>cortex_m4</t>
-  </si>
-  <si>
     <t>isr_func1</t>
   </si>
   <si>
@@ -350,6 +347,9 @@
   </si>
   <si>
     <t>OS_CTX_SAVE_SZ</t>
+  </si>
+  <si>
+    <t>arm926ejs</t>
   </si>
 </sst>
 </file>
@@ -811,19 +811,19 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="73.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" style="5" hidden="1"/>
+    <col min="3" max="3" width="21.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="73.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="5" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -837,7 +837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -845,13 +845,13 @@
         <v>40</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -865,7 +865,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -879,7 +879,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -893,7 +893,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -907,7 +907,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -921,7 +921,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -935,7 +935,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -949,7 +949,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -963,7 +963,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -977,7 +977,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -991,47 +991,47 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C13" s="6">
         <v>512</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C14" s="6">
         <f>32*4</f>
         <v>128</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C15" s="6">
         <v>512</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1065,14 +1065,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.1640625" hidden="1"/>
+    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1104,17 +1104,17 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1128,19 +1128,19 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="68.5" customWidth="1"/>
-    <col min="8" max="16384" width="9.1640625" hidden="1"/>
+    <col min="3" max="3" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="68.42578125" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1157,18 +1157,18 @@
         <v>47</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -1186,7 +1186,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1206,12 +1206,12 @@
         <v>1000</v>
       </c>
       <c r="G3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1222,26 +1222,26 @@
   <dimension ref="A1:K200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5" style="6" customWidth="1"/>
-    <col min="7" max="7" width="11.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.83203125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="27.1640625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="13.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1640625" hidden="1"/>
+    <col min="12" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1270,10 +1270,10 @@
         <v>67</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>35</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>39</v>
@@ -1302,7 +1302,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1360,202 +1360,202 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2"/>
-    <row r="17" x14ac:dyDescent="0.2"/>
-    <row r="18" x14ac:dyDescent="0.2"/>
-    <row r="19" x14ac:dyDescent="0.2"/>
-    <row r="20" x14ac:dyDescent="0.2"/>
-    <row r="21" x14ac:dyDescent="0.2"/>
-    <row r="22" x14ac:dyDescent="0.2"/>
-    <row r="23" x14ac:dyDescent="0.2"/>
-    <row r="24" x14ac:dyDescent="0.2"/>
-    <row r="25" x14ac:dyDescent="0.2"/>
-    <row r="26" x14ac:dyDescent="0.2"/>
-    <row r="27" x14ac:dyDescent="0.2"/>
-    <row r="28" x14ac:dyDescent="0.2"/>
-    <row r="29" x14ac:dyDescent="0.2"/>
-    <row r="30" x14ac:dyDescent="0.2"/>
-    <row r="31" x14ac:dyDescent="0.2"/>
-    <row r="32" x14ac:dyDescent="0.2"/>
-    <row r="33" x14ac:dyDescent="0.2"/>
-    <row r="34" x14ac:dyDescent="0.2"/>
-    <row r="35" x14ac:dyDescent="0.2"/>
-    <row r="36" x14ac:dyDescent="0.2"/>
-    <row r="37" x14ac:dyDescent="0.2"/>
-    <row r="38" x14ac:dyDescent="0.2"/>
-    <row r="39" x14ac:dyDescent="0.2"/>
-    <row r="40" x14ac:dyDescent="0.2"/>
-    <row r="41" x14ac:dyDescent="0.2"/>
-    <row r="42" x14ac:dyDescent="0.2"/>
-    <row r="43" x14ac:dyDescent="0.2"/>
-    <row r="44" x14ac:dyDescent="0.2"/>
-    <row r="45" x14ac:dyDescent="0.2"/>
-    <row r="46" x14ac:dyDescent="0.2"/>
-    <row r="47" x14ac:dyDescent="0.2"/>
-    <row r="48" x14ac:dyDescent="0.2"/>
-    <row r="49" x14ac:dyDescent="0.2"/>
-    <row r="50" x14ac:dyDescent="0.2"/>
-    <row r="51" x14ac:dyDescent="0.2"/>
-    <row r="52" x14ac:dyDescent="0.2"/>
-    <row r="53" x14ac:dyDescent="0.2"/>
-    <row r="54" x14ac:dyDescent="0.2"/>
-    <row r="55" x14ac:dyDescent="0.2"/>
-    <row r="56" x14ac:dyDescent="0.2"/>
-    <row r="57" x14ac:dyDescent="0.2"/>
-    <row r="58" x14ac:dyDescent="0.2"/>
-    <row r="59" x14ac:dyDescent="0.2"/>
-    <row r="60" x14ac:dyDescent="0.2"/>
-    <row r="61" x14ac:dyDescent="0.2"/>
-    <row r="62" x14ac:dyDescent="0.2"/>
-    <row r="63" x14ac:dyDescent="0.2"/>
-    <row r="64" x14ac:dyDescent="0.2"/>
-    <row r="65" x14ac:dyDescent="0.2"/>
-    <row r="66" x14ac:dyDescent="0.2"/>
-    <row r="67" x14ac:dyDescent="0.2"/>
-    <row r="68" x14ac:dyDescent="0.2"/>
-    <row r="69" x14ac:dyDescent="0.2"/>
-    <row r="70" x14ac:dyDescent="0.2"/>
-    <row r="71" x14ac:dyDescent="0.2"/>
-    <row r="72" x14ac:dyDescent="0.2"/>
-    <row r="73" x14ac:dyDescent="0.2"/>
-    <row r="74" x14ac:dyDescent="0.2"/>
-    <row r="75" x14ac:dyDescent="0.2"/>
-    <row r="76" x14ac:dyDescent="0.2"/>
-    <row r="77" x14ac:dyDescent="0.2"/>
-    <row r="78" x14ac:dyDescent="0.2"/>
-    <row r="79" x14ac:dyDescent="0.2"/>
-    <row r="80" x14ac:dyDescent="0.2"/>
-    <row r="81" x14ac:dyDescent="0.2"/>
-    <row r="82" x14ac:dyDescent="0.2"/>
-    <row r="83" x14ac:dyDescent="0.2"/>
-    <row r="84" x14ac:dyDescent="0.2"/>
-    <row r="85" x14ac:dyDescent="0.2"/>
-    <row r="86" x14ac:dyDescent="0.2"/>
-    <row r="87" x14ac:dyDescent="0.2"/>
-    <row r="88" x14ac:dyDescent="0.2"/>
-    <row r="89" x14ac:dyDescent="0.2"/>
-    <row r="90" x14ac:dyDescent="0.2"/>
-    <row r="91" x14ac:dyDescent="0.2"/>
-    <row r="92" x14ac:dyDescent="0.2"/>
-    <row r="93" x14ac:dyDescent="0.2"/>
-    <row r="94" x14ac:dyDescent="0.2"/>
-    <row r="95" x14ac:dyDescent="0.2"/>
-    <row r="96" x14ac:dyDescent="0.2"/>
-    <row r="97" x14ac:dyDescent="0.2"/>
-    <row r="98" x14ac:dyDescent="0.2"/>
-    <row r="99" x14ac:dyDescent="0.2"/>
-    <row r="100" x14ac:dyDescent="0.2"/>
-    <row r="101" x14ac:dyDescent="0.2"/>
-    <row r="102" x14ac:dyDescent="0.2"/>
-    <row r="103" x14ac:dyDescent="0.2"/>
-    <row r="104" x14ac:dyDescent="0.2"/>
-    <row r="105" x14ac:dyDescent="0.2"/>
-    <row r="106" x14ac:dyDescent="0.2"/>
-    <row r="107" x14ac:dyDescent="0.2"/>
-    <row r="108" x14ac:dyDescent="0.2"/>
-    <row r="109" x14ac:dyDescent="0.2"/>
-    <row r="110" x14ac:dyDescent="0.2"/>
-    <row r="111" x14ac:dyDescent="0.2"/>
-    <row r="112" x14ac:dyDescent="0.2"/>
-    <row r="113" x14ac:dyDescent="0.2"/>
-    <row r="114" x14ac:dyDescent="0.2"/>
-    <row r="115" x14ac:dyDescent="0.2"/>
-    <row r="116" x14ac:dyDescent="0.2"/>
-    <row r="117" x14ac:dyDescent="0.2"/>
-    <row r="118" x14ac:dyDescent="0.2"/>
-    <row r="119" x14ac:dyDescent="0.2"/>
-    <row r="120" x14ac:dyDescent="0.2"/>
-    <row r="121" x14ac:dyDescent="0.2"/>
-    <row r="122" x14ac:dyDescent="0.2"/>
-    <row r="123" x14ac:dyDescent="0.2"/>
-    <row r="124" x14ac:dyDescent="0.2"/>
-    <row r="125" x14ac:dyDescent="0.2"/>
-    <row r="126" x14ac:dyDescent="0.2"/>
-    <row r="127" x14ac:dyDescent="0.2"/>
-    <row r="128" x14ac:dyDescent="0.2"/>
-    <row r="129" x14ac:dyDescent="0.2"/>
-    <row r="130" x14ac:dyDescent="0.2"/>
-    <row r="131" x14ac:dyDescent="0.2"/>
-    <row r="132" x14ac:dyDescent="0.2"/>
-    <row r="133" x14ac:dyDescent="0.2"/>
-    <row r="134" x14ac:dyDescent="0.2"/>
-    <row r="135" x14ac:dyDescent="0.2"/>
-    <row r="136" x14ac:dyDescent="0.2"/>
-    <row r="137" x14ac:dyDescent="0.2"/>
-    <row r="138" x14ac:dyDescent="0.2"/>
-    <row r="139" x14ac:dyDescent="0.2"/>
-    <row r="140" x14ac:dyDescent="0.2"/>
-    <row r="141" x14ac:dyDescent="0.2"/>
-    <row r="142" x14ac:dyDescent="0.2"/>
-    <row r="143" x14ac:dyDescent="0.2"/>
-    <row r="144" x14ac:dyDescent="0.2"/>
-    <row r="145" x14ac:dyDescent="0.2"/>
-    <row r="146" x14ac:dyDescent="0.2"/>
-    <row r="147" x14ac:dyDescent="0.2"/>
-    <row r="148" x14ac:dyDescent="0.2"/>
-    <row r="149" x14ac:dyDescent="0.2"/>
-    <row r="150" x14ac:dyDescent="0.2"/>
-    <row r="151" x14ac:dyDescent="0.2"/>
-    <row r="152" x14ac:dyDescent="0.2"/>
-    <row r="153" x14ac:dyDescent="0.2"/>
-    <row r="154" x14ac:dyDescent="0.2"/>
-    <row r="155" x14ac:dyDescent="0.2"/>
-    <row r="156" x14ac:dyDescent="0.2"/>
-    <row r="157" x14ac:dyDescent="0.2"/>
-    <row r="158" x14ac:dyDescent="0.2"/>
-    <row r="159" x14ac:dyDescent="0.2"/>
-    <row r="160" x14ac:dyDescent="0.2"/>
-    <row r="161" x14ac:dyDescent="0.2"/>
-    <row r="162" x14ac:dyDescent="0.2"/>
-    <row r="163" x14ac:dyDescent="0.2"/>
-    <row r="164" x14ac:dyDescent="0.2"/>
-    <row r="165" x14ac:dyDescent="0.2"/>
-    <row r="166" x14ac:dyDescent="0.2"/>
-    <row r="167" x14ac:dyDescent="0.2"/>
-    <row r="168" x14ac:dyDescent="0.2"/>
-    <row r="169" x14ac:dyDescent="0.2"/>
-    <row r="170" x14ac:dyDescent="0.2"/>
-    <row r="171" x14ac:dyDescent="0.2"/>
-    <row r="172" x14ac:dyDescent="0.2"/>
-    <row r="173" x14ac:dyDescent="0.2"/>
-    <row r="174" x14ac:dyDescent="0.2"/>
-    <row r="175" x14ac:dyDescent="0.2"/>
-    <row r="176" x14ac:dyDescent="0.2"/>
-    <row r="177" x14ac:dyDescent="0.2"/>
-    <row r="178" x14ac:dyDescent="0.2"/>
-    <row r="179" x14ac:dyDescent="0.2"/>
-    <row r="180" x14ac:dyDescent="0.2"/>
-    <row r="181" x14ac:dyDescent="0.2"/>
-    <row r="182" x14ac:dyDescent="0.2"/>
-    <row r="183" x14ac:dyDescent="0.2"/>
-    <row r="184" x14ac:dyDescent="0.2"/>
-    <row r="185" x14ac:dyDescent="0.2"/>
-    <row r="186" x14ac:dyDescent="0.2"/>
-    <row r="187" x14ac:dyDescent="0.2"/>
-    <row r="188" x14ac:dyDescent="0.2"/>
-    <row r="189" x14ac:dyDescent="0.2"/>
-    <row r="190" x14ac:dyDescent="0.2"/>
-    <row r="191" x14ac:dyDescent="0.2"/>
-    <row r="192" x14ac:dyDescent="0.2"/>
-    <row r="193" x14ac:dyDescent="0.2"/>
-    <row r="194" x14ac:dyDescent="0.2"/>
-    <row r="195" x14ac:dyDescent="0.2"/>
-    <row r="196" x14ac:dyDescent="0.2"/>
-    <row r="197" x14ac:dyDescent="0.2"/>
-    <row r="198" x14ac:dyDescent="0.2"/>
-    <row r="199" x14ac:dyDescent="0.2"/>
-    <row r="200" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25"/>
+    <row r="17" x14ac:dyDescent="0.25"/>
+    <row r="18" x14ac:dyDescent="0.25"/>
+    <row r="19" x14ac:dyDescent="0.25"/>
+    <row r="20" x14ac:dyDescent="0.25"/>
+    <row r="21" x14ac:dyDescent="0.25"/>
+    <row r="22" x14ac:dyDescent="0.25"/>
+    <row r="23" x14ac:dyDescent="0.25"/>
+    <row r="24" x14ac:dyDescent="0.25"/>
+    <row r="25" x14ac:dyDescent="0.25"/>
+    <row r="26" x14ac:dyDescent="0.25"/>
+    <row r="27" x14ac:dyDescent="0.25"/>
+    <row r="28" x14ac:dyDescent="0.25"/>
+    <row r="29" x14ac:dyDescent="0.25"/>
+    <row r="30" x14ac:dyDescent="0.25"/>
+    <row r="31" x14ac:dyDescent="0.25"/>
+    <row r="32" x14ac:dyDescent="0.25"/>
+    <row r="33" x14ac:dyDescent="0.25"/>
+    <row r="34" x14ac:dyDescent="0.25"/>
+    <row r="35" x14ac:dyDescent="0.25"/>
+    <row r="36" x14ac:dyDescent="0.25"/>
+    <row r="37" x14ac:dyDescent="0.25"/>
+    <row r="38" x14ac:dyDescent="0.25"/>
+    <row r="39" x14ac:dyDescent="0.25"/>
+    <row r="40" x14ac:dyDescent="0.25"/>
+    <row r="41" x14ac:dyDescent="0.25"/>
+    <row r="42" x14ac:dyDescent="0.25"/>
+    <row r="43" x14ac:dyDescent="0.25"/>
+    <row r="44" x14ac:dyDescent="0.25"/>
+    <row r="45" x14ac:dyDescent="0.25"/>
+    <row r="46" x14ac:dyDescent="0.25"/>
+    <row r="47" x14ac:dyDescent="0.25"/>
+    <row r="48" x14ac:dyDescent="0.25"/>
+    <row r="49" x14ac:dyDescent="0.25"/>
+    <row r="50" x14ac:dyDescent="0.25"/>
+    <row r="51" x14ac:dyDescent="0.25"/>
+    <row r="52" x14ac:dyDescent="0.25"/>
+    <row r="53" x14ac:dyDescent="0.25"/>
+    <row r="54" x14ac:dyDescent="0.25"/>
+    <row r="55" x14ac:dyDescent="0.25"/>
+    <row r="56" x14ac:dyDescent="0.25"/>
+    <row r="57" x14ac:dyDescent="0.25"/>
+    <row r="58" x14ac:dyDescent="0.25"/>
+    <row r="59" x14ac:dyDescent="0.25"/>
+    <row r="60" x14ac:dyDescent="0.25"/>
+    <row r="61" x14ac:dyDescent="0.25"/>
+    <row r="62" x14ac:dyDescent="0.25"/>
+    <row r="63" x14ac:dyDescent="0.25"/>
+    <row r="64" x14ac:dyDescent="0.25"/>
+    <row r="65" x14ac:dyDescent="0.25"/>
+    <row r="66" x14ac:dyDescent="0.25"/>
+    <row r="67" x14ac:dyDescent="0.25"/>
+    <row r="68" x14ac:dyDescent="0.25"/>
+    <row r="69" x14ac:dyDescent="0.25"/>
+    <row r="70" x14ac:dyDescent="0.25"/>
+    <row r="71" x14ac:dyDescent="0.25"/>
+    <row r="72" x14ac:dyDescent="0.25"/>
+    <row r="73" x14ac:dyDescent="0.25"/>
+    <row r="74" x14ac:dyDescent="0.25"/>
+    <row r="75" x14ac:dyDescent="0.25"/>
+    <row r="76" x14ac:dyDescent="0.25"/>
+    <row r="77" x14ac:dyDescent="0.25"/>
+    <row r="78" x14ac:dyDescent="0.25"/>
+    <row r="79" x14ac:dyDescent="0.25"/>
+    <row r="80" x14ac:dyDescent="0.25"/>
+    <row r="81" x14ac:dyDescent="0.25"/>
+    <row r="82" x14ac:dyDescent="0.25"/>
+    <row r="83" x14ac:dyDescent="0.25"/>
+    <row r="84" x14ac:dyDescent="0.25"/>
+    <row r="85" x14ac:dyDescent="0.25"/>
+    <row r="86" x14ac:dyDescent="0.25"/>
+    <row r="87" x14ac:dyDescent="0.25"/>
+    <row r="88" x14ac:dyDescent="0.25"/>
+    <row r="89" x14ac:dyDescent="0.25"/>
+    <row r="90" x14ac:dyDescent="0.25"/>
+    <row r="91" x14ac:dyDescent="0.25"/>
+    <row r="92" x14ac:dyDescent="0.25"/>
+    <row r="93" x14ac:dyDescent="0.25"/>
+    <row r="94" x14ac:dyDescent="0.25"/>
+    <row r="95" x14ac:dyDescent="0.25"/>
+    <row r="96" x14ac:dyDescent="0.25"/>
+    <row r="97" x14ac:dyDescent="0.25"/>
+    <row r="98" x14ac:dyDescent="0.25"/>
+    <row r="99" x14ac:dyDescent="0.25"/>
+    <row r="100" x14ac:dyDescent="0.25"/>
+    <row r="101" x14ac:dyDescent="0.25"/>
+    <row r="102" x14ac:dyDescent="0.25"/>
+    <row r="103" x14ac:dyDescent="0.25"/>
+    <row r="104" x14ac:dyDescent="0.25"/>
+    <row r="105" x14ac:dyDescent="0.25"/>
+    <row r="106" x14ac:dyDescent="0.25"/>
+    <row r="107" x14ac:dyDescent="0.25"/>
+    <row r="108" x14ac:dyDescent="0.25"/>
+    <row r="109" x14ac:dyDescent="0.25"/>
+    <row r="110" x14ac:dyDescent="0.25"/>
+    <row r="111" x14ac:dyDescent="0.25"/>
+    <row r="112" x14ac:dyDescent="0.25"/>
+    <row r="113" x14ac:dyDescent="0.25"/>
+    <row r="114" x14ac:dyDescent="0.25"/>
+    <row r="115" x14ac:dyDescent="0.25"/>
+    <row r="116" x14ac:dyDescent="0.25"/>
+    <row r="117" x14ac:dyDescent="0.25"/>
+    <row r="118" x14ac:dyDescent="0.25"/>
+    <row r="119" x14ac:dyDescent="0.25"/>
+    <row r="120" x14ac:dyDescent="0.25"/>
+    <row r="121" x14ac:dyDescent="0.25"/>
+    <row r="122" x14ac:dyDescent="0.25"/>
+    <row r="123" x14ac:dyDescent="0.25"/>
+    <row r="124" x14ac:dyDescent="0.25"/>
+    <row r="125" x14ac:dyDescent="0.25"/>
+    <row r="126" x14ac:dyDescent="0.25"/>
+    <row r="127" x14ac:dyDescent="0.25"/>
+    <row r="128" x14ac:dyDescent="0.25"/>
+    <row r="129" x14ac:dyDescent="0.25"/>
+    <row r="130" x14ac:dyDescent="0.25"/>
+    <row r="131" x14ac:dyDescent="0.25"/>
+    <row r="132" x14ac:dyDescent="0.25"/>
+    <row r="133" x14ac:dyDescent="0.25"/>
+    <row r="134" x14ac:dyDescent="0.25"/>
+    <row r="135" x14ac:dyDescent="0.25"/>
+    <row r="136" x14ac:dyDescent="0.25"/>
+    <row r="137" x14ac:dyDescent="0.25"/>
+    <row r="138" x14ac:dyDescent="0.25"/>
+    <row r="139" x14ac:dyDescent="0.25"/>
+    <row r="140" x14ac:dyDescent="0.25"/>
+    <row r="141" x14ac:dyDescent="0.25"/>
+    <row r="142" x14ac:dyDescent="0.25"/>
+    <row r="143" x14ac:dyDescent="0.25"/>
+    <row r="144" x14ac:dyDescent="0.25"/>
+    <row r="145" x14ac:dyDescent="0.25"/>
+    <row r="146" x14ac:dyDescent="0.25"/>
+    <row r="147" x14ac:dyDescent="0.25"/>
+    <row r="148" x14ac:dyDescent="0.25"/>
+    <row r="149" x14ac:dyDescent="0.25"/>
+    <row r="150" x14ac:dyDescent="0.25"/>
+    <row r="151" x14ac:dyDescent="0.25"/>
+    <row r="152" x14ac:dyDescent="0.25"/>
+    <row r="153" x14ac:dyDescent="0.25"/>
+    <row r="154" x14ac:dyDescent="0.25"/>
+    <row r="155" x14ac:dyDescent="0.25"/>
+    <row r="156" x14ac:dyDescent="0.25"/>
+    <row r="157" x14ac:dyDescent="0.25"/>
+    <row r="158" x14ac:dyDescent="0.25"/>
+    <row r="159" x14ac:dyDescent="0.25"/>
+    <row r="160" x14ac:dyDescent="0.25"/>
+    <row r="161" x14ac:dyDescent="0.25"/>
+    <row r="162" x14ac:dyDescent="0.25"/>
+    <row r="163" x14ac:dyDescent="0.25"/>
+    <row r="164" x14ac:dyDescent="0.25"/>
+    <row r="165" x14ac:dyDescent="0.25"/>
+    <row r="166" x14ac:dyDescent="0.25"/>
+    <row r="167" x14ac:dyDescent="0.25"/>
+    <row r="168" x14ac:dyDescent="0.25"/>
+    <row r="169" x14ac:dyDescent="0.25"/>
+    <row r="170" x14ac:dyDescent="0.25"/>
+    <row r="171" x14ac:dyDescent="0.25"/>
+    <row r="172" x14ac:dyDescent="0.25"/>
+    <row r="173" x14ac:dyDescent="0.25"/>
+    <row r="174" x14ac:dyDescent="0.25"/>
+    <row r="175" x14ac:dyDescent="0.25"/>
+    <row r="176" x14ac:dyDescent="0.25"/>
+    <row r="177" x14ac:dyDescent="0.25"/>
+    <row r="178" x14ac:dyDescent="0.25"/>
+    <row r="179" x14ac:dyDescent="0.25"/>
+    <row r="180" x14ac:dyDescent="0.25"/>
+    <row r="181" x14ac:dyDescent="0.25"/>
+    <row r="182" x14ac:dyDescent="0.25"/>
+    <row r="183" x14ac:dyDescent="0.25"/>
+    <row r="184" x14ac:dyDescent="0.25"/>
+    <row r="185" x14ac:dyDescent="0.25"/>
+    <row r="186" x14ac:dyDescent="0.25"/>
+    <row r="187" x14ac:dyDescent="0.25"/>
+    <row r="188" x14ac:dyDescent="0.25"/>
+    <row r="189" x14ac:dyDescent="0.25"/>
+    <row r="190" x14ac:dyDescent="0.25"/>
+    <row r="191" x14ac:dyDescent="0.25"/>
+    <row r="192" x14ac:dyDescent="0.25"/>
+    <row r="193" x14ac:dyDescent="0.25"/>
+    <row r="194" x14ac:dyDescent="0.25"/>
+    <row r="195" x14ac:dyDescent="0.25"/>
+    <row r="196" x14ac:dyDescent="0.25"/>
+    <row r="197" x14ac:dyDescent="0.25"/>
+    <row r="198" x14ac:dyDescent="0.25"/>
+    <row r="199" x14ac:dyDescent="0.25"/>
+    <row r="200" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -1582,22 +1582,22 @@
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" customWidth="1"/>
-    <col min="7" max="8" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" customWidth="1"/>
-    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="46.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1640625" hidden="1"/>
+    <col min="1" max="1" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
       <c r="C1" s="11"/>
@@ -1616,7 +1616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1649,7 +1649,7 @@
       </c>
       <c r="K2" s="15"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1730,23 +1730,23 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2"/>
-    <row r="17" x14ac:dyDescent="0.2"/>
-    <row r="18" x14ac:dyDescent="0.2"/>
-    <row r="19" x14ac:dyDescent="0.2"/>
-    <row r="20" x14ac:dyDescent="0.2"/>
-    <row r="21" x14ac:dyDescent="0.2"/>
-    <row r="22" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="17" x14ac:dyDescent="0.25"/>
+    <row r="18" x14ac:dyDescent="0.25"/>
+    <row r="19" x14ac:dyDescent="0.25"/>
+    <row r="20" x14ac:dyDescent="0.25"/>
+    <row r="21" x14ac:dyDescent="0.25"/>
+    <row r="22" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="D1:F1"/>
@@ -1783,18 +1783,18 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="84.6640625" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" hidden="1"/>
+    <col min="3" max="3" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="84.7109375" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1814,12 +1814,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
@@ -1828,205 +1828,205 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2"/>
-    <row r="17" x14ac:dyDescent="0.2"/>
-    <row r="18" x14ac:dyDescent="0.2"/>
-    <row r="19" x14ac:dyDescent="0.2"/>
-    <row r="20" x14ac:dyDescent="0.2"/>
-    <row r="21" x14ac:dyDescent="0.2"/>
-    <row r="22" x14ac:dyDescent="0.2"/>
-    <row r="23" x14ac:dyDescent="0.2"/>
-    <row r="24" x14ac:dyDescent="0.2"/>
-    <row r="25" x14ac:dyDescent="0.2"/>
-    <row r="26" x14ac:dyDescent="0.2"/>
-    <row r="27" x14ac:dyDescent="0.2"/>
-    <row r="28" x14ac:dyDescent="0.2"/>
-    <row r="29" x14ac:dyDescent="0.2"/>
-    <row r="30" x14ac:dyDescent="0.2"/>
-    <row r="31" x14ac:dyDescent="0.2"/>
-    <row r="32" x14ac:dyDescent="0.2"/>
-    <row r="33" x14ac:dyDescent="0.2"/>
-    <row r="34" x14ac:dyDescent="0.2"/>
-    <row r="35" x14ac:dyDescent="0.2"/>
-    <row r="36" x14ac:dyDescent="0.2"/>
-    <row r="37" x14ac:dyDescent="0.2"/>
-    <row r="38" x14ac:dyDescent="0.2"/>
-    <row r="39" x14ac:dyDescent="0.2"/>
-    <row r="40" x14ac:dyDescent="0.2"/>
-    <row r="41" x14ac:dyDescent="0.2"/>
-    <row r="42" x14ac:dyDescent="0.2"/>
-    <row r="43" x14ac:dyDescent="0.2"/>
-    <row r="44" x14ac:dyDescent="0.2"/>
-    <row r="45" x14ac:dyDescent="0.2"/>
-    <row r="46" x14ac:dyDescent="0.2"/>
-    <row r="47" x14ac:dyDescent="0.2"/>
-    <row r="48" x14ac:dyDescent="0.2"/>
-    <row r="49" x14ac:dyDescent="0.2"/>
-    <row r="50" x14ac:dyDescent="0.2"/>
-    <row r="51" x14ac:dyDescent="0.2"/>
-    <row r="52" x14ac:dyDescent="0.2"/>
-    <row r="53" x14ac:dyDescent="0.2"/>
-    <row r="54" x14ac:dyDescent="0.2"/>
-    <row r="55" x14ac:dyDescent="0.2"/>
-    <row r="56" x14ac:dyDescent="0.2"/>
-    <row r="57" x14ac:dyDescent="0.2"/>
-    <row r="58" x14ac:dyDescent="0.2"/>
-    <row r="59" x14ac:dyDescent="0.2"/>
-    <row r="60" x14ac:dyDescent="0.2"/>
-    <row r="61" x14ac:dyDescent="0.2"/>
-    <row r="62" x14ac:dyDescent="0.2"/>
-    <row r="63" x14ac:dyDescent="0.2"/>
-    <row r="64" x14ac:dyDescent="0.2"/>
-    <row r="65" x14ac:dyDescent="0.2"/>
-    <row r="66" x14ac:dyDescent="0.2"/>
-    <row r="67" x14ac:dyDescent="0.2"/>
-    <row r="68" x14ac:dyDescent="0.2"/>
-    <row r="69" x14ac:dyDescent="0.2"/>
-    <row r="70" x14ac:dyDescent="0.2"/>
-    <row r="71" x14ac:dyDescent="0.2"/>
-    <row r="72" x14ac:dyDescent="0.2"/>
-    <row r="73" x14ac:dyDescent="0.2"/>
-    <row r="74" x14ac:dyDescent="0.2"/>
-    <row r="75" x14ac:dyDescent="0.2"/>
-    <row r="76" x14ac:dyDescent="0.2"/>
-    <row r="77" x14ac:dyDescent="0.2"/>
-    <row r="78" x14ac:dyDescent="0.2"/>
-    <row r="79" x14ac:dyDescent="0.2"/>
-    <row r="80" x14ac:dyDescent="0.2"/>
-    <row r="81" x14ac:dyDescent="0.2"/>
-    <row r="82" x14ac:dyDescent="0.2"/>
-    <row r="83" x14ac:dyDescent="0.2"/>
-    <row r="84" x14ac:dyDescent="0.2"/>
-    <row r="85" x14ac:dyDescent="0.2"/>
-    <row r="86" x14ac:dyDescent="0.2"/>
-    <row r="87" x14ac:dyDescent="0.2"/>
-    <row r="88" x14ac:dyDescent="0.2"/>
-    <row r="89" x14ac:dyDescent="0.2"/>
-    <row r="90" x14ac:dyDescent="0.2"/>
-    <row r="91" x14ac:dyDescent="0.2"/>
-    <row r="92" x14ac:dyDescent="0.2"/>
-    <row r="93" x14ac:dyDescent="0.2"/>
-    <row r="94" x14ac:dyDescent="0.2"/>
-    <row r="95" x14ac:dyDescent="0.2"/>
-    <row r="96" x14ac:dyDescent="0.2"/>
-    <row r="97" x14ac:dyDescent="0.2"/>
-    <row r="98" x14ac:dyDescent="0.2"/>
-    <row r="99" x14ac:dyDescent="0.2"/>
-    <row r="100" x14ac:dyDescent="0.2"/>
-    <row r="101" x14ac:dyDescent="0.2"/>
-    <row r="102" x14ac:dyDescent="0.2"/>
-    <row r="103" x14ac:dyDescent="0.2"/>
-    <row r="104" x14ac:dyDescent="0.2"/>
-    <row r="105" x14ac:dyDescent="0.2"/>
-    <row r="106" x14ac:dyDescent="0.2"/>
-    <row r="107" x14ac:dyDescent="0.2"/>
-    <row r="108" x14ac:dyDescent="0.2"/>
-    <row r="109" x14ac:dyDescent="0.2"/>
-    <row r="110" x14ac:dyDescent="0.2"/>
-    <row r="111" x14ac:dyDescent="0.2"/>
-    <row r="112" x14ac:dyDescent="0.2"/>
-    <row r="113" x14ac:dyDescent="0.2"/>
-    <row r="114" x14ac:dyDescent="0.2"/>
-    <row r="115" x14ac:dyDescent="0.2"/>
-    <row r="116" x14ac:dyDescent="0.2"/>
-    <row r="117" x14ac:dyDescent="0.2"/>
-    <row r="118" x14ac:dyDescent="0.2"/>
-    <row r="119" x14ac:dyDescent="0.2"/>
-    <row r="120" x14ac:dyDescent="0.2"/>
-    <row r="121" x14ac:dyDescent="0.2"/>
-    <row r="122" x14ac:dyDescent="0.2"/>
-    <row r="123" x14ac:dyDescent="0.2"/>
-    <row r="124" x14ac:dyDescent="0.2"/>
-    <row r="125" x14ac:dyDescent="0.2"/>
-    <row r="126" x14ac:dyDescent="0.2"/>
-    <row r="127" x14ac:dyDescent="0.2"/>
-    <row r="128" x14ac:dyDescent="0.2"/>
-    <row r="129" x14ac:dyDescent="0.2"/>
-    <row r="130" x14ac:dyDescent="0.2"/>
-    <row r="131" x14ac:dyDescent="0.2"/>
-    <row r="132" x14ac:dyDescent="0.2"/>
-    <row r="133" x14ac:dyDescent="0.2"/>
-    <row r="134" x14ac:dyDescent="0.2"/>
-    <row r="135" x14ac:dyDescent="0.2"/>
-    <row r="136" x14ac:dyDescent="0.2"/>
-    <row r="137" x14ac:dyDescent="0.2"/>
-    <row r="138" x14ac:dyDescent="0.2"/>
-    <row r="139" x14ac:dyDescent="0.2"/>
-    <row r="140" x14ac:dyDescent="0.2"/>
-    <row r="141" x14ac:dyDescent="0.2"/>
-    <row r="142" x14ac:dyDescent="0.2"/>
-    <row r="143" x14ac:dyDescent="0.2"/>
-    <row r="144" x14ac:dyDescent="0.2"/>
-    <row r="145" x14ac:dyDescent="0.2"/>
-    <row r="146" x14ac:dyDescent="0.2"/>
-    <row r="147" x14ac:dyDescent="0.2"/>
-    <row r="148" x14ac:dyDescent="0.2"/>
-    <row r="149" x14ac:dyDescent="0.2"/>
-    <row r="150" x14ac:dyDescent="0.2"/>
-    <row r="151" x14ac:dyDescent="0.2"/>
-    <row r="152" x14ac:dyDescent="0.2"/>
-    <row r="153" x14ac:dyDescent="0.2"/>
-    <row r="154" x14ac:dyDescent="0.2"/>
-    <row r="155" x14ac:dyDescent="0.2"/>
-    <row r="156" x14ac:dyDescent="0.2"/>
-    <row r="157" x14ac:dyDescent="0.2"/>
-    <row r="158" x14ac:dyDescent="0.2"/>
-    <row r="159" x14ac:dyDescent="0.2"/>
-    <row r="160" x14ac:dyDescent="0.2"/>
-    <row r="161" x14ac:dyDescent="0.2"/>
-    <row r="162" x14ac:dyDescent="0.2"/>
-    <row r="163" x14ac:dyDescent="0.2"/>
-    <row r="164" x14ac:dyDescent="0.2"/>
-    <row r="165" x14ac:dyDescent="0.2"/>
-    <row r="166" x14ac:dyDescent="0.2"/>
-    <row r="167" x14ac:dyDescent="0.2"/>
-    <row r="168" x14ac:dyDescent="0.2"/>
-    <row r="169" x14ac:dyDescent="0.2"/>
-    <row r="170" x14ac:dyDescent="0.2"/>
-    <row r="171" x14ac:dyDescent="0.2"/>
-    <row r="172" x14ac:dyDescent="0.2"/>
-    <row r="173" x14ac:dyDescent="0.2"/>
-    <row r="174" x14ac:dyDescent="0.2"/>
-    <row r="175" x14ac:dyDescent="0.2"/>
-    <row r="176" x14ac:dyDescent="0.2"/>
-    <row r="177" x14ac:dyDescent="0.2"/>
-    <row r="178" x14ac:dyDescent="0.2"/>
-    <row r="179" x14ac:dyDescent="0.2"/>
-    <row r="180" x14ac:dyDescent="0.2"/>
-    <row r="181" x14ac:dyDescent="0.2"/>
-    <row r="182" x14ac:dyDescent="0.2"/>
-    <row r="183" x14ac:dyDescent="0.2"/>
-    <row r="184" x14ac:dyDescent="0.2"/>
-    <row r="185" x14ac:dyDescent="0.2"/>
-    <row r="186" x14ac:dyDescent="0.2"/>
-    <row r="187" x14ac:dyDescent="0.2"/>
-    <row r="188" x14ac:dyDescent="0.2"/>
-    <row r="189" x14ac:dyDescent="0.2"/>
-    <row r="190" x14ac:dyDescent="0.2"/>
-    <row r="191" x14ac:dyDescent="0.2"/>
-    <row r="192" x14ac:dyDescent="0.2"/>
-    <row r="193" x14ac:dyDescent="0.2"/>
-    <row r="194" x14ac:dyDescent="0.2"/>
-    <row r="195" x14ac:dyDescent="0.2"/>
-    <row r="196" x14ac:dyDescent="0.2"/>
-    <row r="197" x14ac:dyDescent="0.2"/>
-    <row r="198" x14ac:dyDescent="0.2"/>
-    <row r="199" x14ac:dyDescent="0.2"/>
-    <row r="200" x14ac:dyDescent="0.2"/>
-    <row r="201" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="17" x14ac:dyDescent="0.25"/>
+    <row r="18" x14ac:dyDescent="0.25"/>
+    <row r="19" x14ac:dyDescent="0.25"/>
+    <row r="20" x14ac:dyDescent="0.25"/>
+    <row r="21" x14ac:dyDescent="0.25"/>
+    <row r="22" x14ac:dyDescent="0.25"/>
+    <row r="23" x14ac:dyDescent="0.25"/>
+    <row r="24" x14ac:dyDescent="0.25"/>
+    <row r="25" x14ac:dyDescent="0.25"/>
+    <row r="26" x14ac:dyDescent="0.25"/>
+    <row r="27" x14ac:dyDescent="0.25"/>
+    <row r="28" x14ac:dyDescent="0.25"/>
+    <row r="29" x14ac:dyDescent="0.25"/>
+    <row r="30" x14ac:dyDescent="0.25"/>
+    <row r="31" x14ac:dyDescent="0.25"/>
+    <row r="32" x14ac:dyDescent="0.25"/>
+    <row r="33" x14ac:dyDescent="0.25"/>
+    <row r="34" x14ac:dyDescent="0.25"/>
+    <row r="35" x14ac:dyDescent="0.25"/>
+    <row r="36" x14ac:dyDescent="0.25"/>
+    <row r="37" x14ac:dyDescent="0.25"/>
+    <row r="38" x14ac:dyDescent="0.25"/>
+    <row r="39" x14ac:dyDescent="0.25"/>
+    <row r="40" x14ac:dyDescent="0.25"/>
+    <row r="41" x14ac:dyDescent="0.25"/>
+    <row r="42" x14ac:dyDescent="0.25"/>
+    <row r="43" x14ac:dyDescent="0.25"/>
+    <row r="44" x14ac:dyDescent="0.25"/>
+    <row r="45" x14ac:dyDescent="0.25"/>
+    <row r="46" x14ac:dyDescent="0.25"/>
+    <row r="47" x14ac:dyDescent="0.25"/>
+    <row r="48" x14ac:dyDescent="0.25"/>
+    <row r="49" x14ac:dyDescent="0.25"/>
+    <row r="50" x14ac:dyDescent="0.25"/>
+    <row r="51" x14ac:dyDescent="0.25"/>
+    <row r="52" x14ac:dyDescent="0.25"/>
+    <row r="53" x14ac:dyDescent="0.25"/>
+    <row r="54" x14ac:dyDescent="0.25"/>
+    <row r="55" x14ac:dyDescent="0.25"/>
+    <row r="56" x14ac:dyDescent="0.25"/>
+    <row r="57" x14ac:dyDescent="0.25"/>
+    <row r="58" x14ac:dyDescent="0.25"/>
+    <row r="59" x14ac:dyDescent="0.25"/>
+    <row r="60" x14ac:dyDescent="0.25"/>
+    <row r="61" x14ac:dyDescent="0.25"/>
+    <row r="62" x14ac:dyDescent="0.25"/>
+    <row r="63" x14ac:dyDescent="0.25"/>
+    <row r="64" x14ac:dyDescent="0.25"/>
+    <row r="65" x14ac:dyDescent="0.25"/>
+    <row r="66" x14ac:dyDescent="0.25"/>
+    <row r="67" x14ac:dyDescent="0.25"/>
+    <row r="68" x14ac:dyDescent="0.25"/>
+    <row r="69" x14ac:dyDescent="0.25"/>
+    <row r="70" x14ac:dyDescent="0.25"/>
+    <row r="71" x14ac:dyDescent="0.25"/>
+    <row r="72" x14ac:dyDescent="0.25"/>
+    <row r="73" x14ac:dyDescent="0.25"/>
+    <row r="74" x14ac:dyDescent="0.25"/>
+    <row r="75" x14ac:dyDescent="0.25"/>
+    <row r="76" x14ac:dyDescent="0.25"/>
+    <row r="77" x14ac:dyDescent="0.25"/>
+    <row r="78" x14ac:dyDescent="0.25"/>
+    <row r="79" x14ac:dyDescent="0.25"/>
+    <row r="80" x14ac:dyDescent="0.25"/>
+    <row r="81" x14ac:dyDescent="0.25"/>
+    <row r="82" x14ac:dyDescent="0.25"/>
+    <row r="83" x14ac:dyDescent="0.25"/>
+    <row r="84" x14ac:dyDescent="0.25"/>
+    <row r="85" x14ac:dyDescent="0.25"/>
+    <row r="86" x14ac:dyDescent="0.25"/>
+    <row r="87" x14ac:dyDescent="0.25"/>
+    <row r="88" x14ac:dyDescent="0.25"/>
+    <row r="89" x14ac:dyDescent="0.25"/>
+    <row r="90" x14ac:dyDescent="0.25"/>
+    <row r="91" x14ac:dyDescent="0.25"/>
+    <row r="92" x14ac:dyDescent="0.25"/>
+    <row r="93" x14ac:dyDescent="0.25"/>
+    <row r="94" x14ac:dyDescent="0.25"/>
+    <row r="95" x14ac:dyDescent="0.25"/>
+    <row r="96" x14ac:dyDescent="0.25"/>
+    <row r="97" x14ac:dyDescent="0.25"/>
+    <row r="98" x14ac:dyDescent="0.25"/>
+    <row r="99" x14ac:dyDescent="0.25"/>
+    <row r="100" x14ac:dyDescent="0.25"/>
+    <row r="101" x14ac:dyDescent="0.25"/>
+    <row r="102" x14ac:dyDescent="0.25"/>
+    <row r="103" x14ac:dyDescent="0.25"/>
+    <row r="104" x14ac:dyDescent="0.25"/>
+    <row r="105" x14ac:dyDescent="0.25"/>
+    <row r="106" x14ac:dyDescent="0.25"/>
+    <row r="107" x14ac:dyDescent="0.25"/>
+    <row r="108" x14ac:dyDescent="0.25"/>
+    <row r="109" x14ac:dyDescent="0.25"/>
+    <row r="110" x14ac:dyDescent="0.25"/>
+    <row r="111" x14ac:dyDescent="0.25"/>
+    <row r="112" x14ac:dyDescent="0.25"/>
+    <row r="113" x14ac:dyDescent="0.25"/>
+    <row r="114" x14ac:dyDescent="0.25"/>
+    <row r="115" x14ac:dyDescent="0.25"/>
+    <row r="116" x14ac:dyDescent="0.25"/>
+    <row r="117" x14ac:dyDescent="0.25"/>
+    <row r="118" x14ac:dyDescent="0.25"/>
+    <row r="119" x14ac:dyDescent="0.25"/>
+    <row r="120" x14ac:dyDescent="0.25"/>
+    <row r="121" x14ac:dyDescent="0.25"/>
+    <row r="122" x14ac:dyDescent="0.25"/>
+    <row r="123" x14ac:dyDescent="0.25"/>
+    <row r="124" x14ac:dyDescent="0.25"/>
+    <row r="125" x14ac:dyDescent="0.25"/>
+    <row r="126" x14ac:dyDescent="0.25"/>
+    <row r="127" x14ac:dyDescent="0.25"/>
+    <row r="128" x14ac:dyDescent="0.25"/>
+    <row r="129" x14ac:dyDescent="0.25"/>
+    <row r="130" x14ac:dyDescent="0.25"/>
+    <row r="131" x14ac:dyDescent="0.25"/>
+    <row r="132" x14ac:dyDescent="0.25"/>
+    <row r="133" x14ac:dyDescent="0.25"/>
+    <row r="134" x14ac:dyDescent="0.25"/>
+    <row r="135" x14ac:dyDescent="0.25"/>
+    <row r="136" x14ac:dyDescent="0.25"/>
+    <row r="137" x14ac:dyDescent="0.25"/>
+    <row r="138" x14ac:dyDescent="0.25"/>
+    <row r="139" x14ac:dyDescent="0.25"/>
+    <row r="140" x14ac:dyDescent="0.25"/>
+    <row r="141" x14ac:dyDescent="0.25"/>
+    <row r="142" x14ac:dyDescent="0.25"/>
+    <row r="143" x14ac:dyDescent="0.25"/>
+    <row r="144" x14ac:dyDescent="0.25"/>
+    <row r="145" x14ac:dyDescent="0.25"/>
+    <row r="146" x14ac:dyDescent="0.25"/>
+    <row r="147" x14ac:dyDescent="0.25"/>
+    <row r="148" x14ac:dyDescent="0.25"/>
+    <row r="149" x14ac:dyDescent="0.25"/>
+    <row r="150" x14ac:dyDescent="0.25"/>
+    <row r="151" x14ac:dyDescent="0.25"/>
+    <row r="152" x14ac:dyDescent="0.25"/>
+    <row r="153" x14ac:dyDescent="0.25"/>
+    <row r="154" x14ac:dyDescent="0.25"/>
+    <row r="155" x14ac:dyDescent="0.25"/>
+    <row r="156" x14ac:dyDescent="0.25"/>
+    <row r="157" x14ac:dyDescent="0.25"/>
+    <row r="158" x14ac:dyDescent="0.25"/>
+    <row r="159" x14ac:dyDescent="0.25"/>
+    <row r="160" x14ac:dyDescent="0.25"/>
+    <row r="161" x14ac:dyDescent="0.25"/>
+    <row r="162" x14ac:dyDescent="0.25"/>
+    <row r="163" x14ac:dyDescent="0.25"/>
+    <row r="164" x14ac:dyDescent="0.25"/>
+    <row r="165" x14ac:dyDescent="0.25"/>
+    <row r="166" x14ac:dyDescent="0.25"/>
+    <row r="167" x14ac:dyDescent="0.25"/>
+    <row r="168" x14ac:dyDescent="0.25"/>
+    <row r="169" x14ac:dyDescent="0.25"/>
+    <row r="170" x14ac:dyDescent="0.25"/>
+    <row r="171" x14ac:dyDescent="0.25"/>
+    <row r="172" x14ac:dyDescent="0.25"/>
+    <row r="173" x14ac:dyDescent="0.25"/>
+    <row r="174" x14ac:dyDescent="0.25"/>
+    <row r="175" x14ac:dyDescent="0.25"/>
+    <row r="176" x14ac:dyDescent="0.25"/>
+    <row r="177" x14ac:dyDescent="0.25"/>
+    <row r="178" x14ac:dyDescent="0.25"/>
+    <row r="179" x14ac:dyDescent="0.25"/>
+    <row r="180" x14ac:dyDescent="0.25"/>
+    <row r="181" x14ac:dyDescent="0.25"/>
+    <row r="182" x14ac:dyDescent="0.25"/>
+    <row r="183" x14ac:dyDescent="0.25"/>
+    <row r="184" x14ac:dyDescent="0.25"/>
+    <row r="185" x14ac:dyDescent="0.25"/>
+    <row r="186" x14ac:dyDescent="0.25"/>
+    <row r="187" x14ac:dyDescent="0.25"/>
+    <row r="188" x14ac:dyDescent="0.25"/>
+    <row r="189" x14ac:dyDescent="0.25"/>
+    <row r="190" x14ac:dyDescent="0.25"/>
+    <row r="191" x14ac:dyDescent="0.25"/>
+    <row r="192" x14ac:dyDescent="0.25"/>
+    <row r="193" x14ac:dyDescent="0.25"/>
+    <row r="194" x14ac:dyDescent="0.25"/>
+    <row r="195" x14ac:dyDescent="0.25"/>
+    <row r="196" x14ac:dyDescent="0.25"/>
+    <row r="197" x14ac:dyDescent="0.25"/>
+    <row r="198" x14ac:dyDescent="0.25"/>
+    <row r="199" x14ac:dyDescent="0.25"/>
+    <row r="200" x14ac:dyDescent="0.25"/>
+    <row r="201" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2040,15 +2040,15 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.1640625" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
Added infrastructure setup for Ceiling Priority Protocol
Modified the System Generator to identify the ceiling priority from the
input configuration for each resource. Also added additional task to
test the protcol in future.
</commit_message>
<xml_diff>
--- a/tools/OSEK-Builder.xlsx
+++ b/tools/OSEK-Builder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\oss\FreeOSEK\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7872A60-F555-4D3C-BE3D-4DBD0945F3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965663B3-AACF-4650-B8F1-2F55AF097D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="95">
   <si>
     <t>S.No</t>
   </si>
@@ -350,6 +350,15 @@
   </si>
   <si>
     <t>arm926ejs</t>
+  </si>
+  <si>
+    <t>Task_D</t>
+  </si>
+  <si>
+    <t>WakeTaskD</t>
+  </si>
+  <si>
+    <t>To test priority ceiling (Task A vs Task D)</t>
   </si>
 </sst>
 </file>
@@ -482,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -528,6 +537,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -810,7 +820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1221,8 +1231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E239873-4C3E-401B-A75E-3BFB38EFA871}">
   <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1299,7 +1309,7 @@
         <v>39</v>
       </c>
       <c r="J2" s="6">
-        <v>1024</v>
+        <v>512</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1310,7 +1320,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>23</v>
@@ -1319,7 +1329,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>37</v>
@@ -1328,7 +1338,7 @@
         <v>39</v>
       </c>
       <c r="J3" s="6">
-        <v>1024</v>
+        <v>512</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1339,7 +1349,7 @@
         <v>29</v>
       </c>
       <c r="C4" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>23</v>
@@ -1357,10 +1367,32 @@
         <v>38</v>
       </c>
       <c r="J4" s="6">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="6">
+        <v>4</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="6">
+        <v>512</v>
+      </c>
+    </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25"/>
@@ -1579,7 +1611,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1730,7 +1762,38 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>40</v>
+      </c>
+      <c r="I6">
+        <v>1000</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>94</v>
+      </c>
+    </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ISR functions and configuration support is supported now.
Only Timer0 ISR is tested and supported. Others will be done on need
basis.
</commit_message>
<xml_diff>
--- a/tools/OSEK-Builder.xlsx
+++ b/tools/OSEK-Builder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\oss\FreeOSEK\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965663B3-AACF-4650-B8F1-2F55AF097D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57A6CD2-1D37-42C5-8119-300464112089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="96">
   <si>
     <t>S.No</t>
   </si>
@@ -319,9 +319,6 @@
     <t>Category 1 don't use OS service (except interrupt enable/disable), but 2 can use OS services.</t>
   </si>
   <si>
-    <t>isr_func1</t>
-  </si>
-  <si>
     <t>This will be used by the users for delays and usec count</t>
   </si>
   <si>
@@ -359,6 +356,12 @@
   </si>
   <si>
     <t>To test priority ceiling (Task A vs Task D)</t>
+  </si>
+  <si>
+    <t>IRQn</t>
+  </si>
+  <si>
+    <t>SystemTickISR</t>
   </si>
 </sst>
 </file>
@@ -525,6 +528,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -537,7 +541,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -855,7 +858,7 @@
         <v>40</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>41</v>
@@ -1006,13 +1009,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C13" s="6">
         <v>512</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1020,14 +1023,14 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C14" s="6">
         <f>32*4</f>
         <v>128</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1035,13 +1038,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C15" s="6">
         <v>512</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1167,7 +1170,7 @@
         <v>47</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -1178,7 +1181,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -1216,7 +1219,7 @@
         <v>1000</v>
       </c>
       <c r="G3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -1231,7 +1234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E239873-4C3E-401B-A75E-3BFB38EFA871}">
   <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1280,7 +1283,7 @@
         <v>67</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1375,7 +1378,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C5" s="6">
         <v>4</v>
@@ -1633,18 +1636,18 @@
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
       <c r="C1" s="11"/>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="15" t="s">
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="16" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1679,7 +1682,7 @@
       <c r="J2" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="K2" s="15"/>
+      <c r="K2" s="16"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -1767,7 +1770,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -1775,8 +1778,8 @@
       <c r="D6" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="19" t="s">
-        <v>92</v>
+      <c r="E6" s="15" t="s">
+        <v>91</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -1791,7 +1794,7 @@
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25"/>
@@ -1840,71 +1843,78 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F7B285A-14DA-46B0-A287-0CFC1CA6530A}">
-  <dimension ref="A1:F201"/>
+  <dimension ref="A1:G201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="84.7109375" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" hidden="1"/>
+    <col min="3" max="3" width="6.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="84.7109375" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="2">
+        <v>95</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25"/>
     <row r="17" x14ac:dyDescent="0.25"/>
     <row r="18" x14ac:dyDescent="0.25"/>
     <row r="19" x14ac:dyDescent="0.25"/>
@@ -2092,6 +2102,7 @@
     <row r="201" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Adding support for stm32f407vet6 board.
Note: this is a work-in-progress. The current commit is tested for
basic initialization sequence of the OSEK os. But the timer and other
board specific porting is in progress.
</commit_message>
<xml_diff>
--- a/tools/OSEK-Builder.xlsx
+++ b/tools/OSEK-Builder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\oss\FreeOSEK\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57A6CD2-1D37-42C5-8119-300464112089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC04A12E-03C0-49F0-AFE6-394425770232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS" sheetId="1" r:id="rId1"/>
@@ -824,7 +824,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1075,7 +1075,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1138,7 +1138,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1235,7 +1235,7 @@
   <dimension ref="A1:K200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1613,8 +1613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5079921A-7EDA-4A3F-B050-2BF08026BFFC}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1707,7 +1707,7 @@
         <v>40</v>
       </c>
       <c r="I3">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J3" t="s">
         <v>68</v>
@@ -1845,8 +1845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F7B285A-14DA-46B0-A287-0CFC1CA6530A}">
   <dimension ref="A1:G201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
GUI now can read OS info from OIL file
</commit_message>
<xml_diff>
--- a/tools/OSEK-Builder.xlsx
+++ b/tools/OSEK-Builder.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\oss\FreeOSEK\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_E\projects\oss\FreeOSEK\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC04A12E-03C0-49F0-AFE6-394425770232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18801A2F-D596-4ED5-AD6B-3976E7CEFAB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-4344" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OS" sheetId="1" r:id="rId1"/>
@@ -346,9 +346,6 @@
     <t>OS_CTX_SAVE_SZ</t>
   </si>
   <si>
-    <t>arm926ejs</t>
-  </si>
-  <si>
     <t>Task_D</t>
   </si>
   <si>
@@ -362,6 +359,9 @@
   </si>
   <si>
     <t>SystemTickISR</t>
+  </si>
+  <si>
+    <t>cortex-m4</t>
   </si>
 </sst>
 </file>
@@ -823,20 +823,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="73.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="5" hidden="1"/>
+    <col min="3" max="3" width="21.109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="73.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="5" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -850,7 +850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -858,13 +858,13 @@
         <v>40</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -878,7 +878,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -892,7 +892,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -906,7 +906,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -920,7 +920,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -934,7 +934,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -948,7 +948,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -962,7 +962,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -976,7 +976,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -990,7 +990,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1078,14 +1078,14 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" hidden="1"/>
+    <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1117,17 +1117,17 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1141,19 +1141,19 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="68.42578125" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" hidden="1"/>
+    <col min="3" max="3" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="68.44140625" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1222,9 +1222,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1238,23 +1238,23 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.85546875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="27.140625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.88671875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="27.109375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" hidden="1"/>
+    <col min="12" max="16384" width="9.109375" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1373,12 +1373,12 @@
         <v>512</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" s="6">
         <v>4</v>
@@ -1396,201 +1396,201 @@
         <v>512</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25"/>
-    <row r="17" x14ac:dyDescent="0.25"/>
-    <row r="18" x14ac:dyDescent="0.25"/>
-    <row r="19" x14ac:dyDescent="0.25"/>
-    <row r="20" x14ac:dyDescent="0.25"/>
-    <row r="21" x14ac:dyDescent="0.25"/>
-    <row r="22" x14ac:dyDescent="0.25"/>
-    <row r="23" x14ac:dyDescent="0.25"/>
-    <row r="24" x14ac:dyDescent="0.25"/>
-    <row r="25" x14ac:dyDescent="0.25"/>
-    <row r="26" x14ac:dyDescent="0.25"/>
-    <row r="27" x14ac:dyDescent="0.25"/>
-    <row r="28" x14ac:dyDescent="0.25"/>
-    <row r="29" x14ac:dyDescent="0.25"/>
-    <row r="30" x14ac:dyDescent="0.25"/>
-    <row r="31" x14ac:dyDescent="0.25"/>
-    <row r="32" x14ac:dyDescent="0.25"/>
-    <row r="33" x14ac:dyDescent="0.25"/>
-    <row r="34" x14ac:dyDescent="0.25"/>
-    <row r="35" x14ac:dyDescent="0.25"/>
-    <row r="36" x14ac:dyDescent="0.25"/>
-    <row r="37" x14ac:dyDescent="0.25"/>
-    <row r="38" x14ac:dyDescent="0.25"/>
-    <row r="39" x14ac:dyDescent="0.25"/>
-    <row r="40" x14ac:dyDescent="0.25"/>
-    <row r="41" x14ac:dyDescent="0.25"/>
-    <row r="42" x14ac:dyDescent="0.25"/>
-    <row r="43" x14ac:dyDescent="0.25"/>
-    <row r="44" x14ac:dyDescent="0.25"/>
-    <row r="45" x14ac:dyDescent="0.25"/>
-    <row r="46" x14ac:dyDescent="0.25"/>
-    <row r="47" x14ac:dyDescent="0.25"/>
-    <row r="48" x14ac:dyDescent="0.25"/>
-    <row r="49" x14ac:dyDescent="0.25"/>
-    <row r="50" x14ac:dyDescent="0.25"/>
-    <row r="51" x14ac:dyDescent="0.25"/>
-    <row r="52" x14ac:dyDescent="0.25"/>
-    <row r="53" x14ac:dyDescent="0.25"/>
-    <row r="54" x14ac:dyDescent="0.25"/>
-    <row r="55" x14ac:dyDescent="0.25"/>
-    <row r="56" x14ac:dyDescent="0.25"/>
-    <row r="57" x14ac:dyDescent="0.25"/>
-    <row r="58" x14ac:dyDescent="0.25"/>
-    <row r="59" x14ac:dyDescent="0.25"/>
-    <row r="60" x14ac:dyDescent="0.25"/>
-    <row r="61" x14ac:dyDescent="0.25"/>
-    <row r="62" x14ac:dyDescent="0.25"/>
-    <row r="63" x14ac:dyDescent="0.25"/>
-    <row r="64" x14ac:dyDescent="0.25"/>
-    <row r="65" x14ac:dyDescent="0.25"/>
-    <row r="66" x14ac:dyDescent="0.25"/>
-    <row r="67" x14ac:dyDescent="0.25"/>
-    <row r="68" x14ac:dyDescent="0.25"/>
-    <row r="69" x14ac:dyDescent="0.25"/>
-    <row r="70" x14ac:dyDescent="0.25"/>
-    <row r="71" x14ac:dyDescent="0.25"/>
-    <row r="72" x14ac:dyDescent="0.25"/>
-    <row r="73" x14ac:dyDescent="0.25"/>
-    <row r="74" x14ac:dyDescent="0.25"/>
-    <row r="75" x14ac:dyDescent="0.25"/>
-    <row r="76" x14ac:dyDescent="0.25"/>
-    <row r="77" x14ac:dyDescent="0.25"/>
-    <row r="78" x14ac:dyDescent="0.25"/>
-    <row r="79" x14ac:dyDescent="0.25"/>
-    <row r="80" x14ac:dyDescent="0.25"/>
-    <row r="81" x14ac:dyDescent="0.25"/>
-    <row r="82" x14ac:dyDescent="0.25"/>
-    <row r="83" x14ac:dyDescent="0.25"/>
-    <row r="84" x14ac:dyDescent="0.25"/>
-    <row r="85" x14ac:dyDescent="0.25"/>
-    <row r="86" x14ac:dyDescent="0.25"/>
-    <row r="87" x14ac:dyDescent="0.25"/>
-    <row r="88" x14ac:dyDescent="0.25"/>
-    <row r="89" x14ac:dyDescent="0.25"/>
-    <row r="90" x14ac:dyDescent="0.25"/>
-    <row r="91" x14ac:dyDescent="0.25"/>
-    <row r="92" x14ac:dyDescent="0.25"/>
-    <row r="93" x14ac:dyDescent="0.25"/>
-    <row r="94" x14ac:dyDescent="0.25"/>
-    <row r="95" x14ac:dyDescent="0.25"/>
-    <row r="96" x14ac:dyDescent="0.25"/>
-    <row r="97" x14ac:dyDescent="0.25"/>
-    <row r="98" x14ac:dyDescent="0.25"/>
-    <row r="99" x14ac:dyDescent="0.25"/>
-    <row r="100" x14ac:dyDescent="0.25"/>
-    <row r="101" x14ac:dyDescent="0.25"/>
-    <row r="102" x14ac:dyDescent="0.25"/>
-    <row r="103" x14ac:dyDescent="0.25"/>
-    <row r="104" x14ac:dyDescent="0.25"/>
-    <row r="105" x14ac:dyDescent="0.25"/>
-    <row r="106" x14ac:dyDescent="0.25"/>
-    <row r="107" x14ac:dyDescent="0.25"/>
-    <row r="108" x14ac:dyDescent="0.25"/>
-    <row r="109" x14ac:dyDescent="0.25"/>
-    <row r="110" x14ac:dyDescent="0.25"/>
-    <row r="111" x14ac:dyDescent="0.25"/>
-    <row r="112" x14ac:dyDescent="0.25"/>
-    <row r="113" x14ac:dyDescent="0.25"/>
-    <row r="114" x14ac:dyDescent="0.25"/>
-    <row r="115" x14ac:dyDescent="0.25"/>
-    <row r="116" x14ac:dyDescent="0.25"/>
-    <row r="117" x14ac:dyDescent="0.25"/>
-    <row r="118" x14ac:dyDescent="0.25"/>
-    <row r="119" x14ac:dyDescent="0.25"/>
-    <row r="120" x14ac:dyDescent="0.25"/>
-    <row r="121" x14ac:dyDescent="0.25"/>
-    <row r="122" x14ac:dyDescent="0.25"/>
-    <row r="123" x14ac:dyDescent="0.25"/>
-    <row r="124" x14ac:dyDescent="0.25"/>
-    <row r="125" x14ac:dyDescent="0.25"/>
-    <row r="126" x14ac:dyDescent="0.25"/>
-    <row r="127" x14ac:dyDescent="0.25"/>
-    <row r="128" x14ac:dyDescent="0.25"/>
-    <row r="129" x14ac:dyDescent="0.25"/>
-    <row r="130" x14ac:dyDescent="0.25"/>
-    <row r="131" x14ac:dyDescent="0.25"/>
-    <row r="132" x14ac:dyDescent="0.25"/>
-    <row r="133" x14ac:dyDescent="0.25"/>
-    <row r="134" x14ac:dyDescent="0.25"/>
-    <row r="135" x14ac:dyDescent="0.25"/>
-    <row r="136" x14ac:dyDescent="0.25"/>
-    <row r="137" x14ac:dyDescent="0.25"/>
-    <row r="138" x14ac:dyDescent="0.25"/>
-    <row r="139" x14ac:dyDescent="0.25"/>
-    <row r="140" x14ac:dyDescent="0.25"/>
-    <row r="141" x14ac:dyDescent="0.25"/>
-    <row r="142" x14ac:dyDescent="0.25"/>
-    <row r="143" x14ac:dyDescent="0.25"/>
-    <row r="144" x14ac:dyDescent="0.25"/>
-    <row r="145" x14ac:dyDescent="0.25"/>
-    <row r="146" x14ac:dyDescent="0.25"/>
-    <row r="147" x14ac:dyDescent="0.25"/>
-    <row r="148" x14ac:dyDescent="0.25"/>
-    <row r="149" x14ac:dyDescent="0.25"/>
-    <row r="150" x14ac:dyDescent="0.25"/>
-    <row r="151" x14ac:dyDescent="0.25"/>
-    <row r="152" x14ac:dyDescent="0.25"/>
-    <row r="153" x14ac:dyDescent="0.25"/>
-    <row r="154" x14ac:dyDescent="0.25"/>
-    <row r="155" x14ac:dyDescent="0.25"/>
-    <row r="156" x14ac:dyDescent="0.25"/>
-    <row r="157" x14ac:dyDescent="0.25"/>
-    <row r="158" x14ac:dyDescent="0.25"/>
-    <row r="159" x14ac:dyDescent="0.25"/>
-    <row r="160" x14ac:dyDescent="0.25"/>
-    <row r="161" x14ac:dyDescent="0.25"/>
-    <row r="162" x14ac:dyDescent="0.25"/>
-    <row r="163" x14ac:dyDescent="0.25"/>
-    <row r="164" x14ac:dyDescent="0.25"/>
-    <row r="165" x14ac:dyDescent="0.25"/>
-    <row r="166" x14ac:dyDescent="0.25"/>
-    <row r="167" x14ac:dyDescent="0.25"/>
-    <row r="168" x14ac:dyDescent="0.25"/>
-    <row r="169" x14ac:dyDescent="0.25"/>
-    <row r="170" x14ac:dyDescent="0.25"/>
-    <row r="171" x14ac:dyDescent="0.25"/>
-    <row r="172" x14ac:dyDescent="0.25"/>
-    <row r="173" x14ac:dyDescent="0.25"/>
-    <row r="174" x14ac:dyDescent="0.25"/>
-    <row r="175" x14ac:dyDescent="0.25"/>
-    <row r="176" x14ac:dyDescent="0.25"/>
-    <row r="177" x14ac:dyDescent="0.25"/>
-    <row r="178" x14ac:dyDescent="0.25"/>
-    <row r="179" x14ac:dyDescent="0.25"/>
-    <row r="180" x14ac:dyDescent="0.25"/>
-    <row r="181" x14ac:dyDescent="0.25"/>
-    <row r="182" x14ac:dyDescent="0.25"/>
-    <row r="183" x14ac:dyDescent="0.25"/>
-    <row r="184" x14ac:dyDescent="0.25"/>
-    <row r="185" x14ac:dyDescent="0.25"/>
-    <row r="186" x14ac:dyDescent="0.25"/>
-    <row r="187" x14ac:dyDescent="0.25"/>
-    <row r="188" x14ac:dyDescent="0.25"/>
-    <row r="189" x14ac:dyDescent="0.25"/>
-    <row r="190" x14ac:dyDescent="0.25"/>
-    <row r="191" x14ac:dyDescent="0.25"/>
-    <row r="192" x14ac:dyDescent="0.25"/>
-    <row r="193" x14ac:dyDescent="0.25"/>
-    <row r="194" x14ac:dyDescent="0.25"/>
-    <row r="195" x14ac:dyDescent="0.25"/>
-    <row r="196" x14ac:dyDescent="0.25"/>
-    <row r="197" x14ac:dyDescent="0.25"/>
-    <row r="198" x14ac:dyDescent="0.25"/>
-    <row r="199" x14ac:dyDescent="0.25"/>
-    <row r="200" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3"/>
+    <row r="17" x14ac:dyDescent="0.3"/>
+    <row r="18" x14ac:dyDescent="0.3"/>
+    <row r="19" x14ac:dyDescent="0.3"/>
+    <row r="20" x14ac:dyDescent="0.3"/>
+    <row r="21" x14ac:dyDescent="0.3"/>
+    <row r="22" x14ac:dyDescent="0.3"/>
+    <row r="23" x14ac:dyDescent="0.3"/>
+    <row r="24" x14ac:dyDescent="0.3"/>
+    <row r="25" x14ac:dyDescent="0.3"/>
+    <row r="26" x14ac:dyDescent="0.3"/>
+    <row r="27" x14ac:dyDescent="0.3"/>
+    <row r="28" x14ac:dyDescent="0.3"/>
+    <row r="29" x14ac:dyDescent="0.3"/>
+    <row r="30" x14ac:dyDescent="0.3"/>
+    <row r="31" x14ac:dyDescent="0.3"/>
+    <row r="32" x14ac:dyDescent="0.3"/>
+    <row r="33" x14ac:dyDescent="0.3"/>
+    <row r="34" x14ac:dyDescent="0.3"/>
+    <row r="35" x14ac:dyDescent="0.3"/>
+    <row r="36" x14ac:dyDescent="0.3"/>
+    <row r="37" x14ac:dyDescent="0.3"/>
+    <row r="38" x14ac:dyDescent="0.3"/>
+    <row r="39" x14ac:dyDescent="0.3"/>
+    <row r="40" x14ac:dyDescent="0.3"/>
+    <row r="41" x14ac:dyDescent="0.3"/>
+    <row r="42" x14ac:dyDescent="0.3"/>
+    <row r="43" x14ac:dyDescent="0.3"/>
+    <row r="44" x14ac:dyDescent="0.3"/>
+    <row r="45" x14ac:dyDescent="0.3"/>
+    <row r="46" x14ac:dyDescent="0.3"/>
+    <row r="47" x14ac:dyDescent="0.3"/>
+    <row r="48" x14ac:dyDescent="0.3"/>
+    <row r="49" x14ac:dyDescent="0.3"/>
+    <row r="50" x14ac:dyDescent="0.3"/>
+    <row r="51" x14ac:dyDescent="0.3"/>
+    <row r="52" x14ac:dyDescent="0.3"/>
+    <row r="53" x14ac:dyDescent="0.3"/>
+    <row r="54" x14ac:dyDescent="0.3"/>
+    <row r="55" x14ac:dyDescent="0.3"/>
+    <row r="56" x14ac:dyDescent="0.3"/>
+    <row r="57" x14ac:dyDescent="0.3"/>
+    <row r="58" x14ac:dyDescent="0.3"/>
+    <row r="59" x14ac:dyDescent="0.3"/>
+    <row r="60" x14ac:dyDescent="0.3"/>
+    <row r="61" x14ac:dyDescent="0.3"/>
+    <row r="62" x14ac:dyDescent="0.3"/>
+    <row r="63" x14ac:dyDescent="0.3"/>
+    <row r="64" x14ac:dyDescent="0.3"/>
+    <row r="65" x14ac:dyDescent="0.3"/>
+    <row r="66" x14ac:dyDescent="0.3"/>
+    <row r="67" x14ac:dyDescent="0.3"/>
+    <row r="68" x14ac:dyDescent="0.3"/>
+    <row r="69" x14ac:dyDescent="0.3"/>
+    <row r="70" x14ac:dyDescent="0.3"/>
+    <row r="71" x14ac:dyDescent="0.3"/>
+    <row r="72" x14ac:dyDescent="0.3"/>
+    <row r="73" x14ac:dyDescent="0.3"/>
+    <row r="74" x14ac:dyDescent="0.3"/>
+    <row r="75" x14ac:dyDescent="0.3"/>
+    <row r="76" x14ac:dyDescent="0.3"/>
+    <row r="77" x14ac:dyDescent="0.3"/>
+    <row r="78" x14ac:dyDescent="0.3"/>
+    <row r="79" x14ac:dyDescent="0.3"/>
+    <row r="80" x14ac:dyDescent="0.3"/>
+    <row r="81" x14ac:dyDescent="0.3"/>
+    <row r="82" x14ac:dyDescent="0.3"/>
+    <row r="83" x14ac:dyDescent="0.3"/>
+    <row r="84" x14ac:dyDescent="0.3"/>
+    <row r="85" x14ac:dyDescent="0.3"/>
+    <row r="86" x14ac:dyDescent="0.3"/>
+    <row r="87" x14ac:dyDescent="0.3"/>
+    <row r="88" x14ac:dyDescent="0.3"/>
+    <row r="89" x14ac:dyDescent="0.3"/>
+    <row r="90" x14ac:dyDescent="0.3"/>
+    <row r="91" x14ac:dyDescent="0.3"/>
+    <row r="92" x14ac:dyDescent="0.3"/>
+    <row r="93" x14ac:dyDescent="0.3"/>
+    <row r="94" x14ac:dyDescent="0.3"/>
+    <row r="95" x14ac:dyDescent="0.3"/>
+    <row r="96" x14ac:dyDescent="0.3"/>
+    <row r="97" x14ac:dyDescent="0.3"/>
+    <row r="98" x14ac:dyDescent="0.3"/>
+    <row r="99" x14ac:dyDescent="0.3"/>
+    <row r="100" x14ac:dyDescent="0.3"/>
+    <row r="101" x14ac:dyDescent="0.3"/>
+    <row r="102" x14ac:dyDescent="0.3"/>
+    <row r="103" x14ac:dyDescent="0.3"/>
+    <row r="104" x14ac:dyDescent="0.3"/>
+    <row r="105" x14ac:dyDescent="0.3"/>
+    <row r="106" x14ac:dyDescent="0.3"/>
+    <row r="107" x14ac:dyDescent="0.3"/>
+    <row r="108" x14ac:dyDescent="0.3"/>
+    <row r="109" x14ac:dyDescent="0.3"/>
+    <row r="110" x14ac:dyDescent="0.3"/>
+    <row r="111" x14ac:dyDescent="0.3"/>
+    <row r="112" x14ac:dyDescent="0.3"/>
+    <row r="113" x14ac:dyDescent="0.3"/>
+    <row r="114" x14ac:dyDescent="0.3"/>
+    <row r="115" x14ac:dyDescent="0.3"/>
+    <row r="116" x14ac:dyDescent="0.3"/>
+    <row r="117" x14ac:dyDescent="0.3"/>
+    <row r="118" x14ac:dyDescent="0.3"/>
+    <row r="119" x14ac:dyDescent="0.3"/>
+    <row r="120" x14ac:dyDescent="0.3"/>
+    <row r="121" x14ac:dyDescent="0.3"/>
+    <row r="122" x14ac:dyDescent="0.3"/>
+    <row r="123" x14ac:dyDescent="0.3"/>
+    <row r="124" x14ac:dyDescent="0.3"/>
+    <row r="125" x14ac:dyDescent="0.3"/>
+    <row r="126" x14ac:dyDescent="0.3"/>
+    <row r="127" x14ac:dyDescent="0.3"/>
+    <row r="128" x14ac:dyDescent="0.3"/>
+    <row r="129" x14ac:dyDescent="0.3"/>
+    <row r="130" x14ac:dyDescent="0.3"/>
+    <row r="131" x14ac:dyDescent="0.3"/>
+    <row r="132" x14ac:dyDescent="0.3"/>
+    <row r="133" x14ac:dyDescent="0.3"/>
+    <row r="134" x14ac:dyDescent="0.3"/>
+    <row r="135" x14ac:dyDescent="0.3"/>
+    <row r="136" x14ac:dyDescent="0.3"/>
+    <row r="137" x14ac:dyDescent="0.3"/>
+    <row r="138" x14ac:dyDescent="0.3"/>
+    <row r="139" x14ac:dyDescent="0.3"/>
+    <row r="140" x14ac:dyDescent="0.3"/>
+    <row r="141" x14ac:dyDescent="0.3"/>
+    <row r="142" x14ac:dyDescent="0.3"/>
+    <row r="143" x14ac:dyDescent="0.3"/>
+    <row r="144" x14ac:dyDescent="0.3"/>
+    <row r="145" x14ac:dyDescent="0.3"/>
+    <row r="146" x14ac:dyDescent="0.3"/>
+    <row r="147" x14ac:dyDescent="0.3"/>
+    <row r="148" x14ac:dyDescent="0.3"/>
+    <row r="149" x14ac:dyDescent="0.3"/>
+    <row r="150" x14ac:dyDescent="0.3"/>
+    <row r="151" x14ac:dyDescent="0.3"/>
+    <row r="152" x14ac:dyDescent="0.3"/>
+    <row r="153" x14ac:dyDescent="0.3"/>
+    <row r="154" x14ac:dyDescent="0.3"/>
+    <row r="155" x14ac:dyDescent="0.3"/>
+    <row r="156" x14ac:dyDescent="0.3"/>
+    <row r="157" x14ac:dyDescent="0.3"/>
+    <row r="158" x14ac:dyDescent="0.3"/>
+    <row r="159" x14ac:dyDescent="0.3"/>
+    <row r="160" x14ac:dyDescent="0.3"/>
+    <row r="161" x14ac:dyDescent="0.3"/>
+    <row r="162" x14ac:dyDescent="0.3"/>
+    <row r="163" x14ac:dyDescent="0.3"/>
+    <row r="164" x14ac:dyDescent="0.3"/>
+    <row r="165" x14ac:dyDescent="0.3"/>
+    <row r="166" x14ac:dyDescent="0.3"/>
+    <row r="167" x14ac:dyDescent="0.3"/>
+    <row r="168" x14ac:dyDescent="0.3"/>
+    <row r="169" x14ac:dyDescent="0.3"/>
+    <row r="170" x14ac:dyDescent="0.3"/>
+    <row r="171" x14ac:dyDescent="0.3"/>
+    <row r="172" x14ac:dyDescent="0.3"/>
+    <row r="173" x14ac:dyDescent="0.3"/>
+    <row r="174" x14ac:dyDescent="0.3"/>
+    <row r="175" x14ac:dyDescent="0.3"/>
+    <row r="176" x14ac:dyDescent="0.3"/>
+    <row r="177" x14ac:dyDescent="0.3"/>
+    <row r="178" x14ac:dyDescent="0.3"/>
+    <row r="179" x14ac:dyDescent="0.3"/>
+    <row r="180" x14ac:dyDescent="0.3"/>
+    <row r="181" x14ac:dyDescent="0.3"/>
+    <row r="182" x14ac:dyDescent="0.3"/>
+    <row r="183" x14ac:dyDescent="0.3"/>
+    <row r="184" x14ac:dyDescent="0.3"/>
+    <row r="185" x14ac:dyDescent="0.3"/>
+    <row r="186" x14ac:dyDescent="0.3"/>
+    <row r="187" x14ac:dyDescent="0.3"/>
+    <row r="188" x14ac:dyDescent="0.3"/>
+    <row r="189" x14ac:dyDescent="0.3"/>
+    <row r="190" x14ac:dyDescent="0.3"/>
+    <row r="191" x14ac:dyDescent="0.3"/>
+    <row r="192" x14ac:dyDescent="0.3"/>
+    <row r="193" x14ac:dyDescent="0.3"/>
+    <row r="194" x14ac:dyDescent="0.3"/>
+    <row r="195" x14ac:dyDescent="0.3"/>
+    <row r="196" x14ac:dyDescent="0.3"/>
+    <row r="197" x14ac:dyDescent="0.3"/>
+    <row r="198" x14ac:dyDescent="0.3"/>
+    <row r="199" x14ac:dyDescent="0.3"/>
+    <row r="200" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -1613,26 +1613,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5079921A-7EDA-4A3F-B050-2BF08026BFFC}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="46.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" hidden="1"/>
+    <col min="1" max="1" width="5.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" customWidth="1"/>
+    <col min="7" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="46.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
       <c r="C1" s="11"/>
@@ -1651,7 +1651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1684,7 +1684,7 @@
       </c>
       <c r="K2" s="16"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1765,12 +1765,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -1779,7 +1779,7 @@
         <v>56</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -1794,25 +1794,25 @@
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25"/>
-    <row r="17" x14ac:dyDescent="0.25"/>
-    <row r="18" x14ac:dyDescent="0.25"/>
-    <row r="19" x14ac:dyDescent="0.25"/>
-    <row r="20" x14ac:dyDescent="0.25"/>
-    <row r="21" x14ac:dyDescent="0.25"/>
-    <row r="22" x14ac:dyDescent="0.25"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3"/>
+    <row r="17" x14ac:dyDescent="0.3"/>
+    <row r="18" x14ac:dyDescent="0.3"/>
+    <row r="19" x14ac:dyDescent="0.3"/>
+    <row r="20" x14ac:dyDescent="0.3"/>
+    <row r="21" x14ac:dyDescent="0.3"/>
+    <row r="22" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="D1:F1"/>
@@ -1849,19 +1849,19 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="84.7109375" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" hidden="1"/>
+    <col min="3" max="3" width="6.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="84.6640625" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>77</v>
@@ -1884,12 +1884,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -1901,205 +1901,205 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="17" x14ac:dyDescent="0.25"/>
-    <row r="18" x14ac:dyDescent="0.25"/>
-    <row r="19" x14ac:dyDescent="0.25"/>
-    <row r="20" x14ac:dyDescent="0.25"/>
-    <row r="21" x14ac:dyDescent="0.25"/>
-    <row r="22" x14ac:dyDescent="0.25"/>
-    <row r="23" x14ac:dyDescent="0.25"/>
-    <row r="24" x14ac:dyDescent="0.25"/>
-    <row r="25" x14ac:dyDescent="0.25"/>
-    <row r="26" x14ac:dyDescent="0.25"/>
-    <row r="27" x14ac:dyDescent="0.25"/>
-    <row r="28" x14ac:dyDescent="0.25"/>
-    <row r="29" x14ac:dyDescent="0.25"/>
-    <row r="30" x14ac:dyDescent="0.25"/>
-    <row r="31" x14ac:dyDescent="0.25"/>
-    <row r="32" x14ac:dyDescent="0.25"/>
-    <row r="33" x14ac:dyDescent="0.25"/>
-    <row r="34" x14ac:dyDescent="0.25"/>
-    <row r="35" x14ac:dyDescent="0.25"/>
-    <row r="36" x14ac:dyDescent="0.25"/>
-    <row r="37" x14ac:dyDescent="0.25"/>
-    <row r="38" x14ac:dyDescent="0.25"/>
-    <row r="39" x14ac:dyDescent="0.25"/>
-    <row r="40" x14ac:dyDescent="0.25"/>
-    <row r="41" x14ac:dyDescent="0.25"/>
-    <row r="42" x14ac:dyDescent="0.25"/>
-    <row r="43" x14ac:dyDescent="0.25"/>
-    <row r="44" x14ac:dyDescent="0.25"/>
-    <row r="45" x14ac:dyDescent="0.25"/>
-    <row r="46" x14ac:dyDescent="0.25"/>
-    <row r="47" x14ac:dyDescent="0.25"/>
-    <row r="48" x14ac:dyDescent="0.25"/>
-    <row r="49" x14ac:dyDescent="0.25"/>
-    <row r="50" x14ac:dyDescent="0.25"/>
-    <row r="51" x14ac:dyDescent="0.25"/>
-    <row r="52" x14ac:dyDescent="0.25"/>
-    <row r="53" x14ac:dyDescent="0.25"/>
-    <row r="54" x14ac:dyDescent="0.25"/>
-    <row r="55" x14ac:dyDescent="0.25"/>
-    <row r="56" x14ac:dyDescent="0.25"/>
-    <row r="57" x14ac:dyDescent="0.25"/>
-    <row r="58" x14ac:dyDescent="0.25"/>
-    <row r="59" x14ac:dyDescent="0.25"/>
-    <row r="60" x14ac:dyDescent="0.25"/>
-    <row r="61" x14ac:dyDescent="0.25"/>
-    <row r="62" x14ac:dyDescent="0.25"/>
-    <row r="63" x14ac:dyDescent="0.25"/>
-    <row r="64" x14ac:dyDescent="0.25"/>
-    <row r="65" x14ac:dyDescent="0.25"/>
-    <row r="66" x14ac:dyDescent="0.25"/>
-    <row r="67" x14ac:dyDescent="0.25"/>
-    <row r="68" x14ac:dyDescent="0.25"/>
-    <row r="69" x14ac:dyDescent="0.25"/>
-    <row r="70" x14ac:dyDescent="0.25"/>
-    <row r="71" x14ac:dyDescent="0.25"/>
-    <row r="72" x14ac:dyDescent="0.25"/>
-    <row r="73" x14ac:dyDescent="0.25"/>
-    <row r="74" x14ac:dyDescent="0.25"/>
-    <row r="75" x14ac:dyDescent="0.25"/>
-    <row r="76" x14ac:dyDescent="0.25"/>
-    <row r="77" x14ac:dyDescent="0.25"/>
-    <row r="78" x14ac:dyDescent="0.25"/>
-    <row r="79" x14ac:dyDescent="0.25"/>
-    <row r="80" x14ac:dyDescent="0.25"/>
-    <row r="81" x14ac:dyDescent="0.25"/>
-    <row r="82" x14ac:dyDescent="0.25"/>
-    <row r="83" x14ac:dyDescent="0.25"/>
-    <row r="84" x14ac:dyDescent="0.25"/>
-    <row r="85" x14ac:dyDescent="0.25"/>
-    <row r="86" x14ac:dyDescent="0.25"/>
-    <row r="87" x14ac:dyDescent="0.25"/>
-    <row r="88" x14ac:dyDescent="0.25"/>
-    <row r="89" x14ac:dyDescent="0.25"/>
-    <row r="90" x14ac:dyDescent="0.25"/>
-    <row r="91" x14ac:dyDescent="0.25"/>
-    <row r="92" x14ac:dyDescent="0.25"/>
-    <row r="93" x14ac:dyDescent="0.25"/>
-    <row r="94" x14ac:dyDescent="0.25"/>
-    <row r="95" x14ac:dyDescent="0.25"/>
-    <row r="96" x14ac:dyDescent="0.25"/>
-    <row r="97" x14ac:dyDescent="0.25"/>
-    <row r="98" x14ac:dyDescent="0.25"/>
-    <row r="99" x14ac:dyDescent="0.25"/>
-    <row r="100" x14ac:dyDescent="0.25"/>
-    <row r="101" x14ac:dyDescent="0.25"/>
-    <row r="102" x14ac:dyDescent="0.25"/>
-    <row r="103" x14ac:dyDescent="0.25"/>
-    <row r="104" x14ac:dyDescent="0.25"/>
-    <row r="105" x14ac:dyDescent="0.25"/>
-    <row r="106" x14ac:dyDescent="0.25"/>
-    <row r="107" x14ac:dyDescent="0.25"/>
-    <row r="108" x14ac:dyDescent="0.25"/>
-    <row r="109" x14ac:dyDescent="0.25"/>
-    <row r="110" x14ac:dyDescent="0.25"/>
-    <row r="111" x14ac:dyDescent="0.25"/>
-    <row r="112" x14ac:dyDescent="0.25"/>
-    <row r="113" x14ac:dyDescent="0.25"/>
-    <row r="114" x14ac:dyDescent="0.25"/>
-    <row r="115" x14ac:dyDescent="0.25"/>
-    <row r="116" x14ac:dyDescent="0.25"/>
-    <row r="117" x14ac:dyDescent="0.25"/>
-    <row r="118" x14ac:dyDescent="0.25"/>
-    <row r="119" x14ac:dyDescent="0.25"/>
-    <row r="120" x14ac:dyDescent="0.25"/>
-    <row r="121" x14ac:dyDescent="0.25"/>
-    <row r="122" x14ac:dyDescent="0.25"/>
-    <row r="123" x14ac:dyDescent="0.25"/>
-    <row r="124" x14ac:dyDescent="0.25"/>
-    <row r="125" x14ac:dyDescent="0.25"/>
-    <row r="126" x14ac:dyDescent="0.25"/>
-    <row r="127" x14ac:dyDescent="0.25"/>
-    <row r="128" x14ac:dyDescent="0.25"/>
-    <row r="129" x14ac:dyDescent="0.25"/>
-    <row r="130" x14ac:dyDescent="0.25"/>
-    <row r="131" x14ac:dyDescent="0.25"/>
-    <row r="132" x14ac:dyDescent="0.25"/>
-    <row r="133" x14ac:dyDescent="0.25"/>
-    <row r="134" x14ac:dyDescent="0.25"/>
-    <row r="135" x14ac:dyDescent="0.25"/>
-    <row r="136" x14ac:dyDescent="0.25"/>
-    <row r="137" x14ac:dyDescent="0.25"/>
-    <row r="138" x14ac:dyDescent="0.25"/>
-    <row r="139" x14ac:dyDescent="0.25"/>
-    <row r="140" x14ac:dyDescent="0.25"/>
-    <row r="141" x14ac:dyDescent="0.25"/>
-    <row r="142" x14ac:dyDescent="0.25"/>
-    <row r="143" x14ac:dyDescent="0.25"/>
-    <row r="144" x14ac:dyDescent="0.25"/>
-    <row r="145" x14ac:dyDescent="0.25"/>
-    <row r="146" x14ac:dyDescent="0.25"/>
-    <row r="147" x14ac:dyDescent="0.25"/>
-    <row r="148" x14ac:dyDescent="0.25"/>
-    <row r="149" x14ac:dyDescent="0.25"/>
-    <row r="150" x14ac:dyDescent="0.25"/>
-    <row r="151" x14ac:dyDescent="0.25"/>
-    <row r="152" x14ac:dyDescent="0.25"/>
-    <row r="153" x14ac:dyDescent="0.25"/>
-    <row r="154" x14ac:dyDescent="0.25"/>
-    <row r="155" x14ac:dyDescent="0.25"/>
-    <row r="156" x14ac:dyDescent="0.25"/>
-    <row r="157" x14ac:dyDescent="0.25"/>
-    <row r="158" x14ac:dyDescent="0.25"/>
-    <row r="159" x14ac:dyDescent="0.25"/>
-    <row r="160" x14ac:dyDescent="0.25"/>
-    <row r="161" x14ac:dyDescent="0.25"/>
-    <row r="162" x14ac:dyDescent="0.25"/>
-    <row r="163" x14ac:dyDescent="0.25"/>
-    <row r="164" x14ac:dyDescent="0.25"/>
-    <row r="165" x14ac:dyDescent="0.25"/>
-    <row r="166" x14ac:dyDescent="0.25"/>
-    <row r="167" x14ac:dyDescent="0.25"/>
-    <row r="168" x14ac:dyDescent="0.25"/>
-    <row r="169" x14ac:dyDescent="0.25"/>
-    <row r="170" x14ac:dyDescent="0.25"/>
-    <row r="171" x14ac:dyDescent="0.25"/>
-    <row r="172" x14ac:dyDescent="0.25"/>
-    <row r="173" x14ac:dyDescent="0.25"/>
-    <row r="174" x14ac:dyDescent="0.25"/>
-    <row r="175" x14ac:dyDescent="0.25"/>
-    <row r="176" x14ac:dyDescent="0.25"/>
-    <row r="177" x14ac:dyDescent="0.25"/>
-    <row r="178" x14ac:dyDescent="0.25"/>
-    <row r="179" x14ac:dyDescent="0.25"/>
-    <row r="180" x14ac:dyDescent="0.25"/>
-    <row r="181" x14ac:dyDescent="0.25"/>
-    <row r="182" x14ac:dyDescent="0.25"/>
-    <row r="183" x14ac:dyDescent="0.25"/>
-    <row r="184" x14ac:dyDescent="0.25"/>
-    <row r="185" x14ac:dyDescent="0.25"/>
-    <row r="186" x14ac:dyDescent="0.25"/>
-    <row r="187" x14ac:dyDescent="0.25"/>
-    <row r="188" x14ac:dyDescent="0.25"/>
-    <row r="189" x14ac:dyDescent="0.25"/>
-    <row r="190" x14ac:dyDescent="0.25"/>
-    <row r="191" x14ac:dyDescent="0.25"/>
-    <row r="192" x14ac:dyDescent="0.25"/>
-    <row r="193" x14ac:dyDescent="0.25"/>
-    <row r="194" x14ac:dyDescent="0.25"/>
-    <row r="195" x14ac:dyDescent="0.25"/>
-    <row r="196" x14ac:dyDescent="0.25"/>
-    <row r="197" x14ac:dyDescent="0.25"/>
-    <row r="198" x14ac:dyDescent="0.25"/>
-    <row r="199" x14ac:dyDescent="0.25"/>
-    <row r="200" x14ac:dyDescent="0.25"/>
-    <row r="201" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3"/>
+    <row r="17" x14ac:dyDescent="0.3"/>
+    <row r="18" x14ac:dyDescent="0.3"/>
+    <row r="19" x14ac:dyDescent="0.3"/>
+    <row r="20" x14ac:dyDescent="0.3"/>
+    <row r="21" x14ac:dyDescent="0.3"/>
+    <row r="22" x14ac:dyDescent="0.3"/>
+    <row r="23" x14ac:dyDescent="0.3"/>
+    <row r="24" x14ac:dyDescent="0.3"/>
+    <row r="25" x14ac:dyDescent="0.3"/>
+    <row r="26" x14ac:dyDescent="0.3"/>
+    <row r="27" x14ac:dyDescent="0.3"/>
+    <row r="28" x14ac:dyDescent="0.3"/>
+    <row r="29" x14ac:dyDescent="0.3"/>
+    <row r="30" x14ac:dyDescent="0.3"/>
+    <row r="31" x14ac:dyDescent="0.3"/>
+    <row r="32" x14ac:dyDescent="0.3"/>
+    <row r="33" x14ac:dyDescent="0.3"/>
+    <row r="34" x14ac:dyDescent="0.3"/>
+    <row r="35" x14ac:dyDescent="0.3"/>
+    <row r="36" x14ac:dyDescent="0.3"/>
+    <row r="37" x14ac:dyDescent="0.3"/>
+    <row r="38" x14ac:dyDescent="0.3"/>
+    <row r="39" x14ac:dyDescent="0.3"/>
+    <row r="40" x14ac:dyDescent="0.3"/>
+    <row r="41" x14ac:dyDescent="0.3"/>
+    <row r="42" x14ac:dyDescent="0.3"/>
+    <row r="43" x14ac:dyDescent="0.3"/>
+    <row r="44" x14ac:dyDescent="0.3"/>
+    <row r="45" x14ac:dyDescent="0.3"/>
+    <row r="46" x14ac:dyDescent="0.3"/>
+    <row r="47" x14ac:dyDescent="0.3"/>
+    <row r="48" x14ac:dyDescent="0.3"/>
+    <row r="49" x14ac:dyDescent="0.3"/>
+    <row r="50" x14ac:dyDescent="0.3"/>
+    <row r="51" x14ac:dyDescent="0.3"/>
+    <row r="52" x14ac:dyDescent="0.3"/>
+    <row r="53" x14ac:dyDescent="0.3"/>
+    <row r="54" x14ac:dyDescent="0.3"/>
+    <row r="55" x14ac:dyDescent="0.3"/>
+    <row r="56" x14ac:dyDescent="0.3"/>
+    <row r="57" x14ac:dyDescent="0.3"/>
+    <row r="58" x14ac:dyDescent="0.3"/>
+    <row r="59" x14ac:dyDescent="0.3"/>
+    <row r="60" x14ac:dyDescent="0.3"/>
+    <row r="61" x14ac:dyDescent="0.3"/>
+    <row r="62" x14ac:dyDescent="0.3"/>
+    <row r="63" x14ac:dyDescent="0.3"/>
+    <row r="64" x14ac:dyDescent="0.3"/>
+    <row r="65" x14ac:dyDescent="0.3"/>
+    <row r="66" x14ac:dyDescent="0.3"/>
+    <row r="67" x14ac:dyDescent="0.3"/>
+    <row r="68" x14ac:dyDescent="0.3"/>
+    <row r="69" x14ac:dyDescent="0.3"/>
+    <row r="70" x14ac:dyDescent="0.3"/>
+    <row r="71" x14ac:dyDescent="0.3"/>
+    <row r="72" x14ac:dyDescent="0.3"/>
+    <row r="73" x14ac:dyDescent="0.3"/>
+    <row r="74" x14ac:dyDescent="0.3"/>
+    <row r="75" x14ac:dyDescent="0.3"/>
+    <row r="76" x14ac:dyDescent="0.3"/>
+    <row r="77" x14ac:dyDescent="0.3"/>
+    <row r="78" x14ac:dyDescent="0.3"/>
+    <row r="79" x14ac:dyDescent="0.3"/>
+    <row r="80" x14ac:dyDescent="0.3"/>
+    <row r="81" x14ac:dyDescent="0.3"/>
+    <row r="82" x14ac:dyDescent="0.3"/>
+    <row r="83" x14ac:dyDescent="0.3"/>
+    <row r="84" x14ac:dyDescent="0.3"/>
+    <row r="85" x14ac:dyDescent="0.3"/>
+    <row r="86" x14ac:dyDescent="0.3"/>
+    <row r="87" x14ac:dyDescent="0.3"/>
+    <row r="88" x14ac:dyDescent="0.3"/>
+    <row r="89" x14ac:dyDescent="0.3"/>
+    <row r="90" x14ac:dyDescent="0.3"/>
+    <row r="91" x14ac:dyDescent="0.3"/>
+    <row r="92" x14ac:dyDescent="0.3"/>
+    <row r="93" x14ac:dyDescent="0.3"/>
+    <row r="94" x14ac:dyDescent="0.3"/>
+    <row r="95" x14ac:dyDescent="0.3"/>
+    <row r="96" x14ac:dyDescent="0.3"/>
+    <row r="97" x14ac:dyDescent="0.3"/>
+    <row r="98" x14ac:dyDescent="0.3"/>
+    <row r="99" x14ac:dyDescent="0.3"/>
+    <row r="100" x14ac:dyDescent="0.3"/>
+    <row r="101" x14ac:dyDescent="0.3"/>
+    <row r="102" x14ac:dyDescent="0.3"/>
+    <row r="103" x14ac:dyDescent="0.3"/>
+    <row r="104" x14ac:dyDescent="0.3"/>
+    <row r="105" x14ac:dyDescent="0.3"/>
+    <row r="106" x14ac:dyDescent="0.3"/>
+    <row r="107" x14ac:dyDescent="0.3"/>
+    <row r="108" x14ac:dyDescent="0.3"/>
+    <row r="109" x14ac:dyDescent="0.3"/>
+    <row r="110" x14ac:dyDescent="0.3"/>
+    <row r="111" x14ac:dyDescent="0.3"/>
+    <row r="112" x14ac:dyDescent="0.3"/>
+    <row r="113" x14ac:dyDescent="0.3"/>
+    <row r="114" x14ac:dyDescent="0.3"/>
+    <row r="115" x14ac:dyDescent="0.3"/>
+    <row r="116" x14ac:dyDescent="0.3"/>
+    <row r="117" x14ac:dyDescent="0.3"/>
+    <row r="118" x14ac:dyDescent="0.3"/>
+    <row r="119" x14ac:dyDescent="0.3"/>
+    <row r="120" x14ac:dyDescent="0.3"/>
+    <row r="121" x14ac:dyDescent="0.3"/>
+    <row r="122" x14ac:dyDescent="0.3"/>
+    <row r="123" x14ac:dyDescent="0.3"/>
+    <row r="124" x14ac:dyDescent="0.3"/>
+    <row r="125" x14ac:dyDescent="0.3"/>
+    <row r="126" x14ac:dyDescent="0.3"/>
+    <row r="127" x14ac:dyDescent="0.3"/>
+    <row r="128" x14ac:dyDescent="0.3"/>
+    <row r="129" x14ac:dyDescent="0.3"/>
+    <row r="130" x14ac:dyDescent="0.3"/>
+    <row r="131" x14ac:dyDescent="0.3"/>
+    <row r="132" x14ac:dyDescent="0.3"/>
+    <row r="133" x14ac:dyDescent="0.3"/>
+    <row r="134" x14ac:dyDescent="0.3"/>
+    <row r="135" x14ac:dyDescent="0.3"/>
+    <row r="136" x14ac:dyDescent="0.3"/>
+    <row r="137" x14ac:dyDescent="0.3"/>
+    <row r="138" x14ac:dyDescent="0.3"/>
+    <row r="139" x14ac:dyDescent="0.3"/>
+    <row r="140" x14ac:dyDescent="0.3"/>
+    <row r="141" x14ac:dyDescent="0.3"/>
+    <row r="142" x14ac:dyDescent="0.3"/>
+    <row r="143" x14ac:dyDescent="0.3"/>
+    <row r="144" x14ac:dyDescent="0.3"/>
+    <row r="145" x14ac:dyDescent="0.3"/>
+    <row r="146" x14ac:dyDescent="0.3"/>
+    <row r="147" x14ac:dyDescent="0.3"/>
+    <row r="148" x14ac:dyDescent="0.3"/>
+    <row r="149" x14ac:dyDescent="0.3"/>
+    <row r="150" x14ac:dyDescent="0.3"/>
+    <row r="151" x14ac:dyDescent="0.3"/>
+    <row r="152" x14ac:dyDescent="0.3"/>
+    <row r="153" x14ac:dyDescent="0.3"/>
+    <row r="154" x14ac:dyDescent="0.3"/>
+    <row r="155" x14ac:dyDescent="0.3"/>
+    <row r="156" x14ac:dyDescent="0.3"/>
+    <row r="157" x14ac:dyDescent="0.3"/>
+    <row r="158" x14ac:dyDescent="0.3"/>
+    <row r="159" x14ac:dyDescent="0.3"/>
+    <row r="160" x14ac:dyDescent="0.3"/>
+    <row r="161" x14ac:dyDescent="0.3"/>
+    <row r="162" x14ac:dyDescent="0.3"/>
+    <row r="163" x14ac:dyDescent="0.3"/>
+    <row r="164" x14ac:dyDescent="0.3"/>
+    <row r="165" x14ac:dyDescent="0.3"/>
+    <row r="166" x14ac:dyDescent="0.3"/>
+    <row r="167" x14ac:dyDescent="0.3"/>
+    <row r="168" x14ac:dyDescent="0.3"/>
+    <row r="169" x14ac:dyDescent="0.3"/>
+    <row r="170" x14ac:dyDescent="0.3"/>
+    <row r="171" x14ac:dyDescent="0.3"/>
+    <row r="172" x14ac:dyDescent="0.3"/>
+    <row r="173" x14ac:dyDescent="0.3"/>
+    <row r="174" x14ac:dyDescent="0.3"/>
+    <row r="175" x14ac:dyDescent="0.3"/>
+    <row r="176" x14ac:dyDescent="0.3"/>
+    <row r="177" x14ac:dyDescent="0.3"/>
+    <row r="178" x14ac:dyDescent="0.3"/>
+    <row r="179" x14ac:dyDescent="0.3"/>
+    <row r="180" x14ac:dyDescent="0.3"/>
+    <row r="181" x14ac:dyDescent="0.3"/>
+    <row r="182" x14ac:dyDescent="0.3"/>
+    <row r="183" x14ac:dyDescent="0.3"/>
+    <row r="184" x14ac:dyDescent="0.3"/>
+    <row r="185" x14ac:dyDescent="0.3"/>
+    <row r="186" x14ac:dyDescent="0.3"/>
+    <row r="187" x14ac:dyDescent="0.3"/>
+    <row r="188" x14ac:dyDescent="0.3"/>
+    <row r="189" x14ac:dyDescent="0.3"/>
+    <row r="190" x14ac:dyDescent="0.3"/>
+    <row r="191" x14ac:dyDescent="0.3"/>
+    <row r="192" x14ac:dyDescent="0.3"/>
+    <row r="193" x14ac:dyDescent="0.3"/>
+    <row r="194" x14ac:dyDescent="0.3"/>
+    <row r="195" x14ac:dyDescent="0.3"/>
+    <row r="196" x14ac:dyDescent="0.3"/>
+    <row r="197" x14ac:dyDescent="0.3"/>
+    <row r="198" x14ac:dyDescent="0.3"/>
+    <row r="199" x14ac:dyDescent="0.3"/>
+    <row r="200" x14ac:dyDescent="0.3"/>
+    <row r="201" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2114,15 +2114,15 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G4" t="s">
         <v>58</v>
       </c>

</xml_diff>